<commit_message>
Unit Test Day limit checker
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22224" windowHeight="7104" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22224" windowHeight="7104" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="274">
   <si>
     <t>HP_ID</t>
   </si>
@@ -4055,8 +4055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG5"/>
   <sheetViews>
-    <sheetView topLeftCell="DO1" workbookViewId="0">
-      <selection activeCell="DW11" sqref="DW11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4715,7 +4715,7 @@
         <v>999</v>
       </c>
       <c r="B2">
-        <v>611170008</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>20201212</v>
@@ -5017,8 +5017,8 @@
       <c r="DW2">
         <v>6494000</v>
       </c>
-      <c r="DX2" t="s">
-        <v>259</v>
+      <c r="DX2">
+        <v>112</v>
       </c>
       <c r="DY2" t="s">
         <v>259</v>
@@ -6594,7 +6594,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6661,10 +6661,10 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="C2">
-        <v>611170008</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -6709,8 +6709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6743,8 +6743,8 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>259</v>
+      <c r="A2">
+        <v>112</v>
       </c>
       <c r="B2">
         <v>999</v>

</xml_diff>

<commit_message>
Add file Fake Data
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Le Minh\source\repos\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="753" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22230" windowHeight="7110" tabRatio="753" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -19,16 +19,17 @@
     <sheet name="PT_ALRGY_DRUG" sheetId="9" r:id="rId5"/>
     <sheet name="PT_OTHER_DRUG" sheetId="11" r:id="rId6"/>
     <sheet name="TEN_MST" sheetId="12" r:id="rId7"/>
-    <sheet name="KINKI_MST" sheetId="10" r:id="rId8"/>
-    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId9"/>
-    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId10"/>
+    <sheet name="M12_FOOD_ALRGY" sheetId="13" r:id="rId8"/>
+    <sheet name="KINKI_MST" sheetId="10" r:id="rId9"/>
+    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId10"/>
+    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="381">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1150,6 +1151,27 @@
   </si>
   <si>
     <t>6111700T1</t>
+  </si>
+  <si>
+    <t>KIKIN_CD</t>
+  </si>
+  <si>
+    <t>FOOD_KBN</t>
+  </si>
+  <si>
+    <t>ATTENTION_CMT</t>
+  </si>
+  <si>
+    <t>WORKING_MECHANISM</t>
+  </si>
+  <si>
+    <t>7212030S1029</t>
+  </si>
+  <si>
+    <t>・・｢・・ｫ・・ｳ・・ｼ・・ｫ・・ｫ・・・・・・・・ｪ・・｣・・・・・・・・・・・・・・・ｸ・</t>
+  </si>
+  <si>
+    <t>・ｻ・・ｬ・・､・・ｯ・・ｨ・・ｿ・・・・・ｼ・・ｫ・・・・・ｫ・・・・・・・・・・・</t>
   </si>
 </sst>
 </file>
@@ -1982,35 +2004,35 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" customWidth="1"/>
-    <col min="9" max="9" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="46.5546875" customWidth="1"/>
-    <col min="28" max="28" width="28.109375" customWidth="1"/>
-    <col min="29" max="29" width="25.33203125" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1"/>
+    <col min="27" max="27" width="46.5703125" customWidth="1"/>
+    <col min="28" max="28" width="28.140625" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" customWidth="1"/>
     <col min="30" max="30" width="21" customWidth="1"/>
-    <col min="31" max="31" width="18.5546875" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
     <col min="32" max="32" width="28" customWidth="1"/>
-    <col min="33" max="33" width="17.5546875" customWidth="1"/>
-    <col min="34" max="34" width="19.6640625" customWidth="1"/>
-    <col min="35" max="35" width="19.109375" customWidth="1"/>
-    <col min="36" max="36" width="16.109375" customWidth="1"/>
-    <col min="37" max="37" width="16.44140625" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" customWidth="1"/>
+    <col min="34" max="34" width="19.7109375" customWidth="1"/>
+    <col min="35" max="35" width="19.140625" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" customWidth="1"/>
+    <col min="37" max="37" width="16.42578125" customWidth="1"/>
     <col min="38" max="38" width="18" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" customWidth="1"/>
-    <col min="40" max="40" width="14.44140625" customWidth="1"/>
-    <col min="41" max="41" width="14.6640625" customWidth="1"/>
-    <col min="42" max="42" width="34.109375" customWidth="1"/>
-    <col min="44" max="44" width="13.6640625" customWidth="1"/>
-    <col min="45" max="45" width="16.44140625" customWidth="1"/>
-    <col min="47" max="47" width="13.6640625" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" customWidth="1"/>
+    <col min="42" max="42" width="34.140625" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" customWidth="1"/>
+    <col min="45" max="45" width="16.42578125" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47">
@@ -3901,19 +3923,179 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="46" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>999</v>
+      </c>
+      <c r="C2">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45021.481516203705</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45021.48151140046</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>236</v>
+      </c>
+      <c r="M2">
+        <v>20230101</v>
+      </c>
+      <c r="N2">
+        <v>20230301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>999</v>
+      </c>
+      <c r="C3">
+        <v>1234</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45021.481516203705</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45021.48151140046</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>236</v>
+      </c>
+      <c r="M3">
+        <v>20230101</v>
+      </c>
+      <c r="N3">
+        <v>20230301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3977,13 +4159,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4119,16 +4301,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4377,30 +4559,30 @@
       <selection activeCell="BB18" sqref="BB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
-    <col min="5" max="5" width="39.44140625" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" customWidth="1"/>
-    <col min="32" max="32" width="28.5546875" customWidth="1"/>
-    <col min="33" max="33" width="19.88671875" customWidth="1"/>
-    <col min="35" max="35" width="25.33203125" customWidth="1"/>
-    <col min="36" max="36" width="17.88671875" customWidth="1"/>
-    <col min="40" max="40" width="14.5546875" customWidth="1"/>
-    <col min="42" max="42" width="25.33203125" customWidth="1"/>
-    <col min="43" max="43" width="18.33203125" customWidth="1"/>
-    <col min="44" max="44" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" customWidth="1"/>
+    <col min="32" max="32" width="28.5703125" customWidth="1"/>
+    <col min="33" max="33" width="19.85546875" customWidth="1"/>
+    <col min="35" max="35" width="25.28515625" customWidth="1"/>
+    <col min="36" max="36" width="17.85546875" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" customWidth="1"/>
+    <col min="42" max="42" width="25.28515625" customWidth="1"/>
+    <col min="43" max="43" width="18.28515625" customWidth="1"/>
+    <col min="44" max="44" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -4621,24 +4803,24 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="74.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="34.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -4751,16 +4933,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:174">
@@ -4873,11 +5055,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:GG16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:189">
       <c r="A1" t="s">
@@ -12565,95 +12747,52 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="40.200000000000003" customHeight="1">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>374</v>
       </c>
       <c r="B1" t="s">
-        <v>350</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
-        <v>351</v>
+        <v>375</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>259</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>376</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
+        <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45.6" customHeight="1">
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>999</v>
-      </c>
-      <c r="B2">
-        <v>6111</v>
+        <v>610406404</v>
+      </c>
+      <c r="B2" t="s">
+        <v>378</v>
       </c>
       <c r="C2">
-        <v>6404</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45021.481516203705</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" t="s">
-        <v>352</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -12663,157 +12802,95 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
-    <col min="7" max="7" width="46" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:12" ht="40.15" customHeight="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>351</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>237</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:12" ht="45.6" customHeight="1">
       <c r="A2">
-        <v>6</v>
+        <v>999</v>
       </c>
       <c r="B2">
-        <v>999</v>
+        <v>6111</v>
       </c>
       <c r="C2">
-        <v>61</v>
+        <v>6404</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>45021.481516203705</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>2</v>
       </c>
+      <c r="H2" t="s">
+        <v>236</v>
+      </c>
       <c r="I2" t="s">
-        <v>236</v>
-      </c>
-      <c r="J2" s="1">
-        <v>45021.48151140046</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>236</v>
-      </c>
-      <c r="M2">
-        <v>20230101</v>
-      </c>
-      <c r="N2">
-        <v>20230301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>999</v>
-      </c>
-      <c r="C3">
-        <v>1234</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>45021.481516203705</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J3" s="1">
-        <v>45021.48151140046</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>236</v>
-      </c>
-      <c r="M3">
-        <v>20230101</v>
-      </c>
-      <c r="N3">
-        <v>20230301</v>
+        <v>352</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix UnitTest Kinki Test
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="753" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="753" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,16 @@
     <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId10"/>
     <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId11"/>
     <sheet name="M01_KINKI" sheetId="14" r:id="rId12"/>
+    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId13"/>
+    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId14"/>
+    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="396">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1194,6 +1197,30 @@
   </si>
   <si>
     <t>S2001</t>
+  </si>
+  <si>
+    <t>INDEX_CD</t>
+  </si>
+  <si>
+    <t>INDEX_WORD</t>
+  </si>
+  <si>
+    <t>Supple 3</t>
+  </si>
+  <si>
+    <t>UNIT-TEST</t>
+  </si>
+  <si>
+    <t>SEIBUN_CD</t>
+  </si>
+  <si>
+    <t>TOKUHO_FLG</t>
+  </si>
+  <si>
+    <t>UNITTEST</t>
+  </si>
+  <si>
+    <t>UT00002</t>
   </si>
 </sst>
 </file>
@@ -4175,10 +4202,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4232,6 +4259,245 @@
       </c>
       <c r="G2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B3">
+        <v>1190700</v>
+      </c>
+      <c r="C3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D3" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="37.33203125" customWidth="1"/>
+    <col min="10" max="10" width="37.5546875" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>13934</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2" t="s">
+        <v>391</v>
+      </c>
+      <c r="G2">
+        <v>20200101</v>
+      </c>
+      <c r="H2">
+        <v>20231212</v>
+      </c>
+      <c r="I2" t="s">
+        <v>390</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="K5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="K6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="K7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="K8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="K9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="N14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="48.21875" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -5204,11 +5470,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="154" max="154" width="24.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:189">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Fix unit test KinkiOTC Check
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="753" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="926" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,24 @@
     <sheet name="PT_INF" sheetId="8" r:id="rId4"/>
     <sheet name="PT_ALRGY_DRUG" sheetId="9" r:id="rId5"/>
     <sheet name="PT_OTHER_DRUG" sheetId="11" r:id="rId6"/>
-    <sheet name="TEN_MST" sheetId="12" r:id="rId7"/>
-    <sheet name="M12_FOOD_ALRGY" sheetId="13" r:id="rId8"/>
-    <sheet name="KINKI_MST" sheetId="10" r:id="rId9"/>
-    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId10"/>
-    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId11"/>
-    <sheet name="M01_KINKI" sheetId="14" r:id="rId12"/>
-    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId13"/>
-    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId14"/>
-    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId15"/>
+    <sheet name="PT_OTC_DRUG" sheetId="18" r:id="rId7"/>
+    <sheet name="M38_INGREDIENTS" sheetId="19" r:id="rId8"/>
+    <sheet name="TEN_MST" sheetId="12" r:id="rId9"/>
+    <sheet name="M12_FOOD_ALRGY" sheetId="13" r:id="rId10"/>
+    <sheet name="KINKI_MST" sheetId="10" r:id="rId11"/>
+    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId12"/>
+    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId13"/>
+    <sheet name="M01_KINKI" sheetId="14" r:id="rId14"/>
+    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId15"/>
+    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId16"/>
+    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="401">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1221,6 +1223,21 @@
   </si>
   <si>
     <t>UT00002</t>
+  </si>
+  <si>
+    <t>SERIAL_NUM</t>
+  </si>
+  <si>
+    <t>TRADE_NAME</t>
+  </si>
+  <si>
+    <t>・・・・・・・・ｻ・・ｳH2・・</t>
+  </si>
+  <si>
+    <t>UNIT TEST</t>
+  </si>
+  <si>
+    <t>SBT</t>
   </si>
 </sst>
 </file>
@@ -1722,10 +1739,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3972,6 +3990,160 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>610406404</v>
+      </c>
+      <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="40.200000000000003" customHeight="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A2">
+        <v>999</v>
+      </c>
+      <c r="B2">
+        <v>6111</v>
+      </c>
+      <c r="C2">
+        <v>6404</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45021.481516203705</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4130,12 +4302,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4200,12 +4372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4262,8 +4434,8 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>394</v>
+      <c r="A3">
+        <v>9999999</v>
       </c>
       <c r="B3">
         <v>1190700</v>
@@ -4278,6 +4450,26 @@
         <v>3</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>1124</v>
+      </c>
+      <c r="B4">
+        <v>9999999</v>
+      </c>
+      <c r="C4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
@@ -4286,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
@@ -4432,12 +4624,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4470,7 +4662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5307,7 +5499,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5468,9 +5660,203 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="11" max="11" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>999</v>
+      </c>
+      <c r="B2">
+        <v>1231</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>99999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G2">
+        <v>20190603</v>
+      </c>
+      <c r="H2">
+        <v>20231212</v>
+      </c>
+      <c r="I2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>45103.986898148149</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45199.108252777776</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="K3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="K7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="K8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="K11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="K12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3">
+        <v>99999</v>
+      </c>
+      <c r="B2" s="3">
+        <v>9999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -13162,157 +13548,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E1" t="s">
-        <v>376</v>
-      </c>
-      <c r="F1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>610406404</v>
-      </c>
-      <c r="B2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="40.200000000000003" customHeight="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45.6" customHeight="1">
-      <c r="A2">
-        <v>999</v>
-      </c>
-      <c r="B2">
-        <v>6111</v>
-      </c>
-      <c r="C2">
-        <v>6404</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45021.481516203705</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" t="s">
-        <v>352</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Cover Unit Test CheckAge #SMAR-6044
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="926" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="926" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,21 @@
     <sheet name="M38_INGREDIENTS" sheetId="19" r:id="rId9"/>
     <sheet name="TEN_MST" sheetId="12" r:id="rId10"/>
     <sheet name="M12_FOOD_ALRGY" sheetId="13" r:id="rId11"/>
-    <sheet name="KINKI_MST" sheetId="10" r:id="rId12"/>
-    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId13"/>
-    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId14"/>
-    <sheet name="M01_KINKI" sheetId="14" r:id="rId15"/>
-    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId16"/>
-    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId17"/>
-    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId18"/>
+    <sheet name="M14_AGE_CHECK" sheetId="21" r:id="rId12"/>
+    <sheet name="KINKI_MST" sheetId="10" r:id="rId13"/>
+    <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId14"/>
+    <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId15"/>
+    <sheet name="M01_KINKI" sheetId="14" r:id="rId16"/>
+    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId17"/>
+    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId18"/>
+    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="412">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1242,6 +1243,36 @@
   </si>
   <si>
     <t>ALRGY_KBN</t>
+  </si>
+  <si>
+    <t>ATTENTION_CMT_CD</t>
+  </si>
+  <si>
+    <t>AGE_KBN</t>
+  </si>
+  <si>
+    <t>WEIGHT_KBN</t>
+  </si>
+  <si>
+    <t>SEX_KBN</t>
+  </si>
+  <si>
+    <t>AGE_MIN</t>
+  </si>
+  <si>
+    <t>AGE_MAX</t>
+  </si>
+  <si>
+    <t>WEIGHT_MIN</t>
+  </si>
+  <si>
+    <t>WEIGHT_MAX</t>
+  </si>
+  <si>
+    <t>・ｻ・ｸ・・ｬ・・ｫ・ｫ・・ｽ｢・・・・ｧ・・ｯ・・・・・・・ｩ・・・ｽ・・・・ｽ・・ｸ・・・・・・ｦ・・・・・・・・</t>
+  </si>
+  <si>
+    <t>UT</t>
   </si>
 </sst>
 </file>
@@ -1743,11 +1774,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3997,7 +4029,7 @@
   <dimension ref="A1:GG16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11202,7 +11234,7 @@
     </row>
     <row r="16" spans="1:189">
       <c r="A16">
-        <v>999</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>6220816</v>
@@ -11694,7 +11726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -11772,6 +11804,94 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="107.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I1" t="s">
+        <v>407</v>
+      </c>
+      <c r="J1" t="s">
+        <v>408</v>
+      </c>
+      <c r="K1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="4">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>999</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -11870,7 +11990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -12030,7 +12150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -12100,7 +12220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -12206,7 +12326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
@@ -12352,7 +12472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12390,7 +12510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Cover UT check thuoc KinkiUserChecker
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="926" firstSheet="14" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="926" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="424">
   <si>
     <t>HP_ID</t>
   </si>
@@ -4259,10 +4259,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG17"/>
+  <dimension ref="A1:GG19"/>
   <sheetViews>
-    <sheetView topLeftCell="DK1" workbookViewId="0">
-      <selection activeCell="DX17" sqref="DX17"/>
+    <sheetView topLeftCell="DP1" workbookViewId="0">
+      <selection activeCell="EC28" sqref="EC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12432,6 +12432,976 @@
         <v>0</v>
       </c>
       <c r="GG17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:189">
+      <c r="A18">
+        <v>999</v>
+      </c>
+      <c r="B18">
+        <v>6404</v>
+      </c>
+      <c r="C18">
+        <v>20220401</v>
+      </c>
+      <c r="D18">
+        <v>99999999</v>
+      </c>
+      <c r="E18" t="s">
+        <v>230</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>364</v>
+      </c>
+      <c r="H18" t="s">
+        <v>371</v>
+      </c>
+      <c r="P18" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>343</v>
+      </c>
+      <c r="S18">
+        <v>47</v>
+      </c>
+      <c r="T18" t="s">
+        <v>279</v>
+      </c>
+      <c r="U18" t="s">
+        <v>279</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>0</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>0</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BB18">
+        <v>0</v>
+      </c>
+      <c r="BC18">
+        <v>0</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+      <c r="BE18">
+        <v>0</v>
+      </c>
+      <c r="BF18">
+        <v>0</v>
+      </c>
+      <c r="BG18">
+        <v>0</v>
+      </c>
+      <c r="BH18">
+        <v>0</v>
+      </c>
+      <c r="BI18">
+        <v>0</v>
+      </c>
+      <c r="BJ18">
+        <v>0</v>
+      </c>
+      <c r="BK18">
+        <v>0</v>
+      </c>
+      <c r="BL18">
+        <v>0</v>
+      </c>
+      <c r="BM18">
+        <v>0</v>
+      </c>
+      <c r="BN18">
+        <v>0</v>
+      </c>
+      <c r="BO18">
+        <v>0</v>
+      </c>
+      <c r="BP18">
+        <v>0</v>
+      </c>
+      <c r="BQ18">
+        <v>0</v>
+      </c>
+      <c r="BR18">
+        <v>0</v>
+      </c>
+      <c r="BS18">
+        <v>0</v>
+      </c>
+      <c r="BT18">
+        <v>0</v>
+      </c>
+      <c r="BV18">
+        <v>0</v>
+      </c>
+      <c r="BW18">
+        <v>0</v>
+      </c>
+      <c r="BX18">
+        <v>0</v>
+      </c>
+      <c r="BY18">
+        <v>0</v>
+      </c>
+      <c r="BZ18">
+        <v>0</v>
+      </c>
+      <c r="CA18">
+        <v>0</v>
+      </c>
+      <c r="CB18">
+        <v>0</v>
+      </c>
+      <c r="CC18">
+        <v>0</v>
+      </c>
+      <c r="CD18">
+        <v>0</v>
+      </c>
+      <c r="CE18">
+        <v>0</v>
+      </c>
+      <c r="CF18">
+        <v>0</v>
+      </c>
+      <c r="CG18">
+        <v>0</v>
+      </c>
+      <c r="CT18">
+        <v>0</v>
+      </c>
+      <c r="CU18">
+        <v>0</v>
+      </c>
+      <c r="CV18">
+        <v>0</v>
+      </c>
+      <c r="CW18">
+        <v>0</v>
+      </c>
+      <c r="CX18">
+        <v>0</v>
+      </c>
+      <c r="CY18">
+        <v>4</v>
+      </c>
+      <c r="CZ18">
+        <v>0</v>
+      </c>
+      <c r="DA18">
+        <v>0</v>
+      </c>
+      <c r="DB18">
+        <v>0</v>
+      </c>
+      <c r="DC18">
+        <v>0</v>
+      </c>
+      <c r="DD18">
+        <v>0</v>
+      </c>
+      <c r="DE18">
+        <v>0</v>
+      </c>
+      <c r="DF18">
+        <v>0</v>
+      </c>
+      <c r="DG18">
+        <v>0</v>
+      </c>
+      <c r="DH18">
+        <v>0</v>
+      </c>
+      <c r="DJ18">
+        <v>0</v>
+      </c>
+      <c r="DK18">
+        <v>0</v>
+      </c>
+      <c r="DL18">
+        <v>0</v>
+      </c>
+      <c r="DM18">
+        <v>0</v>
+      </c>
+      <c r="DN18">
+        <v>0</v>
+      </c>
+      <c r="DP18">
+        <v>0</v>
+      </c>
+      <c r="DQ18">
+        <v>0</v>
+      </c>
+      <c r="DR18">
+        <v>0</v>
+      </c>
+      <c r="DS18">
+        <v>0</v>
+      </c>
+      <c r="DT18">
+        <v>0</v>
+      </c>
+      <c r="DU18">
+        <v>0</v>
+      </c>
+      <c r="DV18">
+        <v>0</v>
+      </c>
+      <c r="DW18">
+        <v>0</v>
+      </c>
+      <c r="DX18">
+        <v>6404</v>
+      </c>
+      <c r="DY18" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ18">
+        <v>0</v>
+      </c>
+      <c r="EA18">
+        <v>0</v>
+      </c>
+      <c r="EB18">
+        <v>20220401</v>
+      </c>
+      <c r="EC18">
+        <v>99999999</v>
+      </c>
+      <c r="ED18">
+        <v>0</v>
+      </c>
+      <c r="EE18">
+        <v>0</v>
+      </c>
+      <c r="EF18">
+        <v>0</v>
+      </c>
+      <c r="EG18">
+        <v>0</v>
+      </c>
+      <c r="EH18">
+        <v>0</v>
+      </c>
+      <c r="EI18">
+        <v>0</v>
+      </c>
+      <c r="EJ18">
+        <v>0</v>
+      </c>
+      <c r="EK18">
+        <v>0</v>
+      </c>
+      <c r="EL18">
+        <v>0</v>
+      </c>
+      <c r="EM18">
+        <v>0</v>
+      </c>
+      <c r="EN18">
+        <v>0</v>
+      </c>
+      <c r="EO18">
+        <v>0</v>
+      </c>
+      <c r="EP18" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ18">
+        <v>0</v>
+      </c>
+      <c r="ER18">
+        <v>0</v>
+      </c>
+      <c r="ES18">
+        <v>0</v>
+      </c>
+      <c r="ET18">
+        <v>0</v>
+      </c>
+      <c r="EU18">
+        <v>0</v>
+      </c>
+      <c r="EV18">
+        <v>1</v>
+      </c>
+      <c r="EW18">
+        <v>0</v>
+      </c>
+      <c r="EX18">
+        <v>620001936</v>
+      </c>
+      <c r="EY18">
+        <v>0</v>
+      </c>
+      <c r="FA18">
+        <v>0</v>
+      </c>
+      <c r="FD18">
+        <v>0</v>
+      </c>
+      <c r="FE18">
+        <v>0</v>
+      </c>
+      <c r="FF18">
+        <v>0</v>
+      </c>
+      <c r="FG18">
+        <v>0</v>
+      </c>
+      <c r="FH18">
+        <v>0</v>
+      </c>
+      <c r="FI18">
+        <v>0</v>
+      </c>
+      <c r="FJ18">
+        <v>0</v>
+      </c>
+      <c r="FK18">
+        <v>0</v>
+      </c>
+      <c r="FL18">
+        <v>0</v>
+      </c>
+      <c r="FM18">
+        <v>0</v>
+      </c>
+      <c r="FN18">
+        <v>0</v>
+      </c>
+      <c r="FO18" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP18">
+        <v>0</v>
+      </c>
+      <c r="FR18" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS18">
+        <v>0</v>
+      </c>
+      <c r="FU18">
+        <v>0</v>
+      </c>
+      <c r="FV18">
+        <v>0</v>
+      </c>
+      <c r="FW18">
+        <v>0</v>
+      </c>
+      <c r="FX18">
+        <v>0</v>
+      </c>
+      <c r="FY18">
+        <v>0</v>
+      </c>
+      <c r="FZ18">
+        <v>0</v>
+      </c>
+      <c r="GA18">
+        <v>0</v>
+      </c>
+      <c r="GB18">
+        <v>0</v>
+      </c>
+      <c r="GC18">
+        <v>0</v>
+      </c>
+      <c r="GD18">
+        <v>0</v>
+      </c>
+      <c r="GE18">
+        <v>0</v>
+      </c>
+      <c r="GF18">
+        <v>0</v>
+      </c>
+      <c r="GG18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:189">
+      <c r="A19">
+        <v>999</v>
+      </c>
+      <c r="B19">
+        <v>6111</v>
+      </c>
+      <c r="C19">
+        <v>20220401</v>
+      </c>
+      <c r="D19">
+        <v>99999999</v>
+      </c>
+      <c r="E19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>364</v>
+      </c>
+      <c r="H19" t="s">
+        <v>371</v>
+      </c>
+      <c r="P19" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>343</v>
+      </c>
+      <c r="S19">
+        <v>47</v>
+      </c>
+      <c r="T19" t="s">
+        <v>279</v>
+      </c>
+      <c r="U19" t="s">
+        <v>279</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19">
+        <v>0</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19">
+        <v>0</v>
+      </c>
+      <c r="AV19">
+        <v>0</v>
+      </c>
+      <c r="AW19">
+        <v>0</v>
+      </c>
+      <c r="AX19">
+        <v>0</v>
+      </c>
+      <c r="AY19">
+        <v>0</v>
+      </c>
+      <c r="AZ19">
+        <v>0</v>
+      </c>
+      <c r="BA19">
+        <v>0</v>
+      </c>
+      <c r="BB19">
+        <v>0</v>
+      </c>
+      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="BD19">
+        <v>0</v>
+      </c>
+      <c r="BE19">
+        <v>0</v>
+      </c>
+      <c r="BF19">
+        <v>0</v>
+      </c>
+      <c r="BG19">
+        <v>0</v>
+      </c>
+      <c r="BH19">
+        <v>0</v>
+      </c>
+      <c r="BI19">
+        <v>0</v>
+      </c>
+      <c r="BJ19">
+        <v>0</v>
+      </c>
+      <c r="BK19">
+        <v>0</v>
+      </c>
+      <c r="BL19">
+        <v>0</v>
+      </c>
+      <c r="BM19">
+        <v>0</v>
+      </c>
+      <c r="BN19">
+        <v>0</v>
+      </c>
+      <c r="BO19">
+        <v>0</v>
+      </c>
+      <c r="BP19">
+        <v>0</v>
+      </c>
+      <c r="BQ19">
+        <v>0</v>
+      </c>
+      <c r="BR19">
+        <v>0</v>
+      </c>
+      <c r="BS19">
+        <v>0</v>
+      </c>
+      <c r="BT19">
+        <v>0</v>
+      </c>
+      <c r="BV19">
+        <v>0</v>
+      </c>
+      <c r="BW19">
+        <v>0</v>
+      </c>
+      <c r="BX19">
+        <v>0</v>
+      </c>
+      <c r="BY19">
+        <v>0</v>
+      </c>
+      <c r="BZ19">
+        <v>0</v>
+      </c>
+      <c r="CA19">
+        <v>0</v>
+      </c>
+      <c r="CB19">
+        <v>0</v>
+      </c>
+      <c r="CC19">
+        <v>0</v>
+      </c>
+      <c r="CD19">
+        <v>0</v>
+      </c>
+      <c r="CE19">
+        <v>0</v>
+      </c>
+      <c r="CF19">
+        <v>0</v>
+      </c>
+      <c r="CG19">
+        <v>0</v>
+      </c>
+      <c r="CT19">
+        <v>0</v>
+      </c>
+      <c r="CU19">
+        <v>0</v>
+      </c>
+      <c r="CV19">
+        <v>0</v>
+      </c>
+      <c r="CW19">
+        <v>0</v>
+      </c>
+      <c r="CX19">
+        <v>0</v>
+      </c>
+      <c r="CY19">
+        <v>4</v>
+      </c>
+      <c r="CZ19">
+        <v>0</v>
+      </c>
+      <c r="DA19">
+        <v>0</v>
+      </c>
+      <c r="DB19">
+        <v>0</v>
+      </c>
+      <c r="DC19">
+        <v>0</v>
+      </c>
+      <c r="DD19">
+        <v>0</v>
+      </c>
+      <c r="DE19">
+        <v>0</v>
+      </c>
+      <c r="DF19">
+        <v>0</v>
+      </c>
+      <c r="DG19">
+        <v>0</v>
+      </c>
+      <c r="DH19">
+        <v>0</v>
+      </c>
+      <c r="DJ19">
+        <v>0</v>
+      </c>
+      <c r="DK19">
+        <v>0</v>
+      </c>
+      <c r="DL19">
+        <v>0</v>
+      </c>
+      <c r="DM19">
+        <v>0</v>
+      </c>
+      <c r="DN19">
+        <v>0</v>
+      </c>
+      <c r="DP19">
+        <v>0</v>
+      </c>
+      <c r="DQ19">
+        <v>0</v>
+      </c>
+      <c r="DR19">
+        <v>0</v>
+      </c>
+      <c r="DS19">
+        <v>0</v>
+      </c>
+      <c r="DT19">
+        <v>0</v>
+      </c>
+      <c r="DU19">
+        <v>0</v>
+      </c>
+      <c r="DV19">
+        <v>0</v>
+      </c>
+      <c r="DW19">
+        <v>0</v>
+      </c>
+      <c r="DX19">
+        <v>6111</v>
+      </c>
+      <c r="DY19" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ19">
+        <v>0</v>
+      </c>
+      <c r="EA19">
+        <v>0</v>
+      </c>
+      <c r="EB19">
+        <v>20220401</v>
+      </c>
+      <c r="EC19">
+        <v>99999999</v>
+      </c>
+      <c r="ED19">
+        <v>0</v>
+      </c>
+      <c r="EE19">
+        <v>0</v>
+      </c>
+      <c r="EF19">
+        <v>0</v>
+      </c>
+      <c r="EG19">
+        <v>0</v>
+      </c>
+      <c r="EH19">
+        <v>0</v>
+      </c>
+      <c r="EI19">
+        <v>0</v>
+      </c>
+      <c r="EJ19">
+        <v>0</v>
+      </c>
+      <c r="EK19">
+        <v>0</v>
+      </c>
+      <c r="EL19">
+        <v>0</v>
+      </c>
+      <c r="EM19">
+        <v>0</v>
+      </c>
+      <c r="EN19">
+        <v>0</v>
+      </c>
+      <c r="EO19">
+        <v>0</v>
+      </c>
+      <c r="EP19" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ19">
+        <v>0</v>
+      </c>
+      <c r="ER19">
+        <v>0</v>
+      </c>
+      <c r="ES19">
+        <v>0</v>
+      </c>
+      <c r="ET19">
+        <v>0</v>
+      </c>
+      <c r="EU19">
+        <v>0</v>
+      </c>
+      <c r="EV19">
+        <v>1</v>
+      </c>
+      <c r="EW19">
+        <v>0</v>
+      </c>
+      <c r="EX19">
+        <v>620001936</v>
+      </c>
+      <c r="EY19">
+        <v>0</v>
+      </c>
+      <c r="FA19">
+        <v>0</v>
+      </c>
+      <c r="FD19">
+        <v>0</v>
+      </c>
+      <c r="FE19">
+        <v>0</v>
+      </c>
+      <c r="FF19">
+        <v>0</v>
+      </c>
+      <c r="FG19">
+        <v>0</v>
+      </c>
+      <c r="FH19">
+        <v>0</v>
+      </c>
+      <c r="FI19">
+        <v>0</v>
+      </c>
+      <c r="FJ19">
+        <v>0</v>
+      </c>
+      <c r="FK19">
+        <v>0</v>
+      </c>
+      <c r="FL19">
+        <v>0</v>
+      </c>
+      <c r="FM19">
+        <v>0</v>
+      </c>
+      <c r="FN19">
+        <v>0</v>
+      </c>
+      <c r="FO19" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP19">
+        <v>0</v>
+      </c>
+      <c r="FR19" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS19">
+        <v>0</v>
+      </c>
+      <c r="FU19">
+        <v>0</v>
+      </c>
+      <c r="FV19">
+        <v>0</v>
+      </c>
+      <c r="FW19">
+        <v>0</v>
+      </c>
+      <c r="FX19">
+        <v>0</v>
+      </c>
+      <c r="FY19">
+        <v>0</v>
+      </c>
+      <c r="FZ19">
+        <v>0</v>
+      </c>
+      <c r="GA19">
+        <v>0</v>
+      </c>
+      <c r="GB19">
+        <v>0</v>
+      </c>
+      <c r="GC19">
+        <v>0</v>
+      </c>
+      <c r="GD19">
+        <v>0</v>
+      </c>
+      <c r="GE19">
+        <v>0</v>
+      </c>
+      <c r="GF19">
+        <v>0</v>
+      </c>
+      <c r="GG19">
         <v>0</v>
       </c>
     </row>
@@ -12757,10 +13727,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12846,6 +13816,41 @@
         <v>0</v>
       </c>
       <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A3">
+        <v>999</v>
+      </c>
+      <c r="B3">
+        <v>6404</v>
+      </c>
+      <c r="C3">
+        <v>6404</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45021.481516203705</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>236</v>
+      </c>
+      <c r="I3" t="s">
+        <v>352</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>10</v>
       </c>
     </row>
@@ -13088,7 +14093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cover Finder RealtimeCheck UnitTest
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22236" windowHeight="7116" tabRatio="961" firstSheet="11" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="961" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,24 @@
     <sheet name="DRUG_DAY_LIMIT" sheetId="4" r:id="rId17"/>
     <sheet name="M10_DAY_LIMIT" sheetId="5" r:id="rId18"/>
     <sheet name="M56_EX_ED_INGREDIENTS" sheetId="25" r:id="rId19"/>
-    <sheet name="M56_PRODRUG_CD" sheetId="26" r:id="rId20"/>
-    <sheet name="M01_KINKI" sheetId="14" r:id="rId21"/>
-    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId22"/>
-    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId23"/>
-    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId24"/>
+    <sheet name="M56_EX_INGRDT_MAIN" sheetId="27" r:id="rId20"/>
+    <sheet name="M56_ALRGY_DERIVATIVES" sheetId="32" r:id="rId21"/>
+    <sheet name="M56_DRVALRGY_CODE" sheetId="33" r:id="rId22"/>
+    <sheet name="M56_PRODRUG_CD" sheetId="26" r:id="rId23"/>
+    <sheet name="M56_YJ_DRUG_CLASS" sheetId="29" r:id="rId24"/>
+    <sheet name="M56_DRUG_CLASS" sheetId="30" r:id="rId25"/>
+    <sheet name="M56_EX_ANALOGUE" sheetId="31" r:id="rId26"/>
+    <sheet name="M01_KINKI" sheetId="14" r:id="rId27"/>
+    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId28"/>
+    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId29"/>
+    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId30"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="471">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1331,9 +1337,6 @@
     <t>TENKABUTU_CHECK</t>
   </si>
   <si>
-    <t>UT2700X1011</t>
-  </si>
-  <si>
     <t>UT2700</t>
   </si>
   <si>
@@ -1343,10 +1346,121 @@
     <t>IS11230A0</t>
   </si>
   <si>
-    <t>UT2700X1012</t>
-  </si>
-  <si>
     <t>UT2701</t>
+  </si>
+  <si>
+    <t>UT271012</t>
+  </si>
+  <si>
+    <t>UT271011</t>
+  </si>
+  <si>
+    <t>YOHO_CD</t>
+  </si>
+  <si>
+    <t>HAIGOU_FLG</t>
+  </si>
+  <si>
+    <t>YUEKI_FLG</t>
+  </si>
+  <si>
+    <t>KANPO_FLG</t>
+  </si>
+  <si>
+    <t>ZENSINSAYO_FLG</t>
+  </si>
+  <si>
+    <t>USG013</t>
+  </si>
+  <si>
+    <t>UT271013</t>
+  </si>
+  <si>
+    <t>UT271014</t>
+  </si>
+  <si>
+    <t>UT2702</t>
+  </si>
+  <si>
+    <t>UT2703</t>
+  </si>
+  <si>
+    <t>USG014</t>
+  </si>
+  <si>
+    <t>CLASS_CD</t>
+  </si>
+  <si>
+    <t>CLASS_NAME</t>
+  </si>
+  <si>
+    <t>CLASS_DUPLICATION</t>
+  </si>
+  <si>
+    <t>11UT1011</t>
+  </si>
+  <si>
+    <t>11UT1012</t>
+  </si>
+  <si>
+    <t>UT180100</t>
+  </si>
+  <si>
+    <t>UT_CLASS0</t>
+  </si>
+  <si>
+    <t>UT2704</t>
+  </si>
+  <si>
+    <t>UT2705</t>
+  </si>
+  <si>
+    <t>ANALOGUE_CD</t>
+  </si>
+  <si>
+    <t>AL0000024</t>
+  </si>
+  <si>
+    <t>11UT1013</t>
+  </si>
+  <si>
+    <t>USG015</t>
+  </si>
+  <si>
+    <t>11UT1014</t>
+  </si>
+  <si>
+    <t>UT2706</t>
+  </si>
+  <si>
+    <t>UT2707</t>
+  </si>
+  <si>
+    <t>DRVALRGY_CD</t>
+  </si>
+  <si>
+    <t>IS1112700</t>
+  </si>
+  <si>
+    <t>DRVALRGY_NAME</t>
+  </si>
+  <si>
+    <t>DRVALRGY_GRP</t>
+  </si>
+  <si>
+    <t>RANK_NO</t>
+  </si>
+  <si>
+    <t>G001</t>
+  </si>
+  <si>
+    <t>UT000313</t>
+  </si>
+  <si>
+    <t>UT271015</t>
+  </si>
+  <si>
+    <t>UT2708</t>
   </si>
 </sst>
 </file>
@@ -2178,7 +2292,7 @@
   <dimension ref="A1:AU24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4294,10 +4408,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG21"/>
+  <dimension ref="A1:GG28"/>
   <sheetViews>
-    <sheetView topLeftCell="DQ1" workbookViewId="0">
-      <selection activeCell="DX21" sqref="DX21"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="DM1" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="DW28" sqref="DW28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13446,7 +13560,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C20">
         <v>20220401</v>
@@ -13755,7 +13869,7 @@
         <v>0</v>
       </c>
       <c r="DX20" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="DY20" t="s">
         <v>280</v>
@@ -13931,7 +14045,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C21">
         <v>20220401</v>
@@ -14411,8 +14525,3404 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:189">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>443</v>
+      </c>
+      <c r="C22">
+        <v>20220401</v>
+      </c>
+      <c r="D22">
+        <v>99999999</v>
+      </c>
+      <c r="E22" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>364</v>
+      </c>
+      <c r="H22" t="s">
+        <v>371</v>
+      </c>
+      <c r="P22" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>343</v>
+      </c>
+      <c r="S22">
+        <v>47</v>
+      </c>
+      <c r="T22" t="s">
+        <v>279</v>
+      </c>
+      <c r="U22" t="s">
+        <v>279</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22">
+        <v>0</v>
+      </c>
+      <c r="AR22">
+        <v>0</v>
+      </c>
+      <c r="AS22">
+        <v>0</v>
+      </c>
+      <c r="AT22">
+        <v>0</v>
+      </c>
+      <c r="AU22">
+        <v>0</v>
+      </c>
+      <c r="AV22">
+        <v>0</v>
+      </c>
+      <c r="AW22">
+        <v>0</v>
+      </c>
+      <c r="AX22">
+        <v>0</v>
+      </c>
+      <c r="AY22">
+        <v>0</v>
+      </c>
+      <c r="AZ22">
+        <v>0</v>
+      </c>
+      <c r="BA22">
+        <v>0</v>
+      </c>
+      <c r="BB22">
+        <v>0</v>
+      </c>
+      <c r="BC22">
+        <v>0</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+      <c r="BE22">
+        <v>0</v>
+      </c>
+      <c r="BF22">
+        <v>0</v>
+      </c>
+      <c r="BG22">
+        <v>0</v>
+      </c>
+      <c r="BH22">
+        <v>0</v>
+      </c>
+      <c r="BI22">
+        <v>0</v>
+      </c>
+      <c r="BJ22">
+        <v>0</v>
+      </c>
+      <c r="BK22">
+        <v>0</v>
+      </c>
+      <c r="BL22">
+        <v>0</v>
+      </c>
+      <c r="BM22">
+        <v>0</v>
+      </c>
+      <c r="BN22">
+        <v>0</v>
+      </c>
+      <c r="BO22">
+        <v>0</v>
+      </c>
+      <c r="BP22">
+        <v>0</v>
+      </c>
+      <c r="BQ22">
+        <v>0</v>
+      </c>
+      <c r="BR22">
+        <v>0</v>
+      </c>
+      <c r="BS22">
+        <v>0</v>
+      </c>
+      <c r="BT22">
+        <v>0</v>
+      </c>
+      <c r="BV22">
+        <v>0</v>
+      </c>
+      <c r="BW22">
+        <v>0</v>
+      </c>
+      <c r="BX22">
+        <v>0</v>
+      </c>
+      <c r="BY22">
+        <v>0</v>
+      </c>
+      <c r="BZ22">
+        <v>0</v>
+      </c>
+      <c r="CA22">
+        <v>0</v>
+      </c>
+      <c r="CB22">
+        <v>0</v>
+      </c>
+      <c r="CC22">
+        <v>0</v>
+      </c>
+      <c r="CD22">
+        <v>0</v>
+      </c>
+      <c r="CE22">
+        <v>0</v>
+      </c>
+      <c r="CF22">
+        <v>0</v>
+      </c>
+      <c r="CG22">
+        <v>0</v>
+      </c>
+      <c r="CT22">
+        <v>0</v>
+      </c>
+      <c r="CU22">
+        <v>0</v>
+      </c>
+      <c r="CV22">
+        <v>0</v>
+      </c>
+      <c r="CW22">
+        <v>0</v>
+      </c>
+      <c r="CX22">
+        <v>0</v>
+      </c>
+      <c r="CY22">
+        <v>4</v>
+      </c>
+      <c r="CZ22">
+        <v>0</v>
+      </c>
+      <c r="DA22">
+        <v>0</v>
+      </c>
+      <c r="DB22">
+        <v>0</v>
+      </c>
+      <c r="DC22">
+        <v>0</v>
+      </c>
+      <c r="DD22">
+        <v>0</v>
+      </c>
+      <c r="DE22">
+        <v>0</v>
+      </c>
+      <c r="DF22">
+        <v>0</v>
+      </c>
+      <c r="DG22">
+        <v>0</v>
+      </c>
+      <c r="DH22">
+        <v>0</v>
+      </c>
+      <c r="DJ22">
+        <v>0</v>
+      </c>
+      <c r="DK22">
+        <v>0</v>
+      </c>
+      <c r="DL22">
+        <v>0</v>
+      </c>
+      <c r="DM22">
+        <v>0</v>
+      </c>
+      <c r="DN22">
+        <v>0</v>
+      </c>
+      <c r="DP22">
+        <v>0</v>
+      </c>
+      <c r="DQ22">
+        <v>0</v>
+      </c>
+      <c r="DR22">
+        <v>0</v>
+      </c>
+      <c r="DS22">
+        <v>0</v>
+      </c>
+      <c r="DT22">
+        <v>0</v>
+      </c>
+      <c r="DU22">
+        <v>0</v>
+      </c>
+      <c r="DV22">
+        <v>0</v>
+      </c>
+      <c r="DW22">
+        <v>0</v>
+      </c>
+      <c r="DX22" t="s">
+        <v>441</v>
+      </c>
+      <c r="DY22" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ22">
+        <v>0</v>
+      </c>
+      <c r="EA22">
+        <v>0</v>
+      </c>
+      <c r="EB22">
+        <v>20220401</v>
+      </c>
+      <c r="EC22">
+        <v>99999999</v>
+      </c>
+      <c r="ED22">
+        <v>0</v>
+      </c>
+      <c r="EE22">
+        <v>0</v>
+      </c>
+      <c r="EF22">
+        <v>0</v>
+      </c>
+      <c r="EG22">
+        <v>0</v>
+      </c>
+      <c r="EH22">
+        <v>0</v>
+      </c>
+      <c r="EI22">
+        <v>0</v>
+      </c>
+      <c r="EJ22">
+        <v>0</v>
+      </c>
+      <c r="EK22">
+        <v>0</v>
+      </c>
+      <c r="EL22">
+        <v>0</v>
+      </c>
+      <c r="EM22">
+        <v>0</v>
+      </c>
+      <c r="EN22">
+        <v>0</v>
+      </c>
+      <c r="EO22">
+        <v>0</v>
+      </c>
+      <c r="EP22" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ22">
+        <v>0</v>
+      </c>
+      <c r="ER22">
+        <v>0</v>
+      </c>
+      <c r="ES22">
+        <v>0</v>
+      </c>
+      <c r="ET22">
+        <v>0</v>
+      </c>
+      <c r="EU22">
+        <v>0</v>
+      </c>
+      <c r="EV22">
+        <v>1</v>
+      </c>
+      <c r="EW22">
+        <v>0</v>
+      </c>
+      <c r="EX22">
+        <v>620001936</v>
+      </c>
+      <c r="EY22">
+        <v>0</v>
+      </c>
+      <c r="FA22">
+        <v>0</v>
+      </c>
+      <c r="FD22">
+        <v>0</v>
+      </c>
+      <c r="FE22">
+        <v>0</v>
+      </c>
+      <c r="FF22">
+        <v>0</v>
+      </c>
+      <c r="FG22">
+        <v>0</v>
+      </c>
+      <c r="FH22">
+        <v>0</v>
+      </c>
+      <c r="FI22">
+        <v>0</v>
+      </c>
+      <c r="FJ22">
+        <v>0</v>
+      </c>
+      <c r="FK22">
+        <v>0</v>
+      </c>
+      <c r="FL22">
+        <v>0</v>
+      </c>
+      <c r="FM22">
+        <v>0</v>
+      </c>
+      <c r="FN22">
+        <v>0</v>
+      </c>
+      <c r="FO22" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP22">
+        <v>0</v>
+      </c>
+      <c r="FR22" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS22">
+        <v>0</v>
+      </c>
+      <c r="FU22">
+        <v>0</v>
+      </c>
+      <c r="FV22">
+        <v>0</v>
+      </c>
+      <c r="FW22">
+        <v>0</v>
+      </c>
+      <c r="FX22">
+        <v>0</v>
+      </c>
+      <c r="FY22">
+        <v>0</v>
+      </c>
+      <c r="FZ22">
+        <v>0</v>
+      </c>
+      <c r="GA22">
+        <v>0</v>
+      </c>
+      <c r="GB22">
+        <v>0</v>
+      </c>
+      <c r="GC22">
+        <v>0</v>
+      </c>
+      <c r="GD22">
+        <v>0</v>
+      </c>
+      <c r="GE22">
+        <v>0</v>
+      </c>
+      <c r="GF22">
+        <v>0</v>
+      </c>
+      <c r="GG22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:189">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>444</v>
+      </c>
+      <c r="C23">
+        <v>20220401</v>
+      </c>
+      <c r="D23">
+        <v>99999999</v>
+      </c>
+      <c r="E23" t="s">
+        <v>230</v>
+      </c>
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>364</v>
+      </c>
+      <c r="H23" t="s">
+        <v>371</v>
+      </c>
+      <c r="P23" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>343</v>
+      </c>
+      <c r="S23">
+        <v>47</v>
+      </c>
+      <c r="T23" t="s">
+        <v>279</v>
+      </c>
+      <c r="U23" t="s">
+        <v>279</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>0</v>
+      </c>
+      <c r="AW23">
+        <v>0</v>
+      </c>
+      <c r="AX23">
+        <v>0</v>
+      </c>
+      <c r="AY23">
+        <v>0</v>
+      </c>
+      <c r="AZ23">
+        <v>0</v>
+      </c>
+      <c r="BA23">
+        <v>0</v>
+      </c>
+      <c r="BB23">
+        <v>0</v>
+      </c>
+      <c r="BC23">
+        <v>0</v>
+      </c>
+      <c r="BD23">
+        <v>0</v>
+      </c>
+      <c r="BE23">
+        <v>0</v>
+      </c>
+      <c r="BF23">
+        <v>0</v>
+      </c>
+      <c r="BG23">
+        <v>0</v>
+      </c>
+      <c r="BH23">
+        <v>0</v>
+      </c>
+      <c r="BI23">
+        <v>0</v>
+      </c>
+      <c r="BJ23">
+        <v>0</v>
+      </c>
+      <c r="BK23">
+        <v>0</v>
+      </c>
+      <c r="BL23">
+        <v>0</v>
+      </c>
+      <c r="BM23">
+        <v>0</v>
+      </c>
+      <c r="BN23">
+        <v>0</v>
+      </c>
+      <c r="BO23">
+        <v>0</v>
+      </c>
+      <c r="BP23">
+        <v>0</v>
+      </c>
+      <c r="BQ23">
+        <v>0</v>
+      </c>
+      <c r="BR23">
+        <v>0</v>
+      </c>
+      <c r="BS23">
+        <v>0</v>
+      </c>
+      <c r="BT23">
+        <v>0</v>
+      </c>
+      <c r="BV23">
+        <v>0</v>
+      </c>
+      <c r="BW23">
+        <v>0</v>
+      </c>
+      <c r="BX23">
+        <v>0</v>
+      </c>
+      <c r="BY23">
+        <v>0</v>
+      </c>
+      <c r="BZ23">
+        <v>0</v>
+      </c>
+      <c r="CA23">
+        <v>0</v>
+      </c>
+      <c r="CB23">
+        <v>0</v>
+      </c>
+      <c r="CC23">
+        <v>0</v>
+      </c>
+      <c r="CD23">
+        <v>0</v>
+      </c>
+      <c r="CE23">
+        <v>0</v>
+      </c>
+      <c r="CF23">
+        <v>0</v>
+      </c>
+      <c r="CG23">
+        <v>0</v>
+      </c>
+      <c r="CT23">
+        <v>0</v>
+      </c>
+      <c r="CU23">
+        <v>0</v>
+      </c>
+      <c r="CV23">
+        <v>0</v>
+      </c>
+      <c r="CW23">
+        <v>0</v>
+      </c>
+      <c r="CX23">
+        <v>0</v>
+      </c>
+      <c r="CY23">
+        <v>4</v>
+      </c>
+      <c r="CZ23">
+        <v>0</v>
+      </c>
+      <c r="DA23">
+        <v>0</v>
+      </c>
+      <c r="DB23">
+        <v>0</v>
+      </c>
+      <c r="DC23">
+        <v>0</v>
+      </c>
+      <c r="DD23">
+        <v>0</v>
+      </c>
+      <c r="DE23">
+        <v>0</v>
+      </c>
+      <c r="DF23">
+        <v>0</v>
+      </c>
+      <c r="DG23">
+        <v>0</v>
+      </c>
+      <c r="DH23">
+        <v>0</v>
+      </c>
+      <c r="DJ23">
+        <v>0</v>
+      </c>
+      <c r="DK23">
+        <v>0</v>
+      </c>
+      <c r="DL23">
+        <v>0</v>
+      </c>
+      <c r="DM23">
+        <v>0</v>
+      </c>
+      <c r="DN23">
+        <v>0</v>
+      </c>
+      <c r="DP23">
+        <v>0</v>
+      </c>
+      <c r="DQ23">
+        <v>0</v>
+      </c>
+      <c r="DR23">
+        <v>0</v>
+      </c>
+      <c r="DS23">
+        <v>0</v>
+      </c>
+      <c r="DT23">
+        <v>0</v>
+      </c>
+      <c r="DU23">
+        <v>0</v>
+      </c>
+      <c r="DV23">
+        <v>0</v>
+      </c>
+      <c r="DW23">
+        <v>0</v>
+      </c>
+      <c r="DX23" t="s">
+        <v>442</v>
+      </c>
+      <c r="DY23" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ23">
+        <v>0</v>
+      </c>
+      <c r="EA23">
+        <v>0</v>
+      </c>
+      <c r="EB23">
+        <v>20220401</v>
+      </c>
+      <c r="EC23">
+        <v>99999999</v>
+      </c>
+      <c r="ED23">
+        <v>0</v>
+      </c>
+      <c r="EE23">
+        <v>0</v>
+      </c>
+      <c r="EF23">
+        <v>0</v>
+      </c>
+      <c r="EG23">
+        <v>0</v>
+      </c>
+      <c r="EH23">
+        <v>0</v>
+      </c>
+      <c r="EI23">
+        <v>0</v>
+      </c>
+      <c r="EJ23">
+        <v>0</v>
+      </c>
+      <c r="EK23">
+        <v>0</v>
+      </c>
+      <c r="EL23">
+        <v>0</v>
+      </c>
+      <c r="EM23">
+        <v>0</v>
+      </c>
+      <c r="EN23">
+        <v>0</v>
+      </c>
+      <c r="EO23">
+        <v>0</v>
+      </c>
+      <c r="EP23" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ23">
+        <v>0</v>
+      </c>
+      <c r="ER23">
+        <v>0</v>
+      </c>
+      <c r="ES23">
+        <v>0</v>
+      </c>
+      <c r="ET23">
+        <v>0</v>
+      </c>
+      <c r="EU23">
+        <v>0</v>
+      </c>
+      <c r="EV23">
+        <v>1</v>
+      </c>
+      <c r="EW23">
+        <v>0</v>
+      </c>
+      <c r="EX23">
+        <v>620001936</v>
+      </c>
+      <c r="EY23">
+        <v>0</v>
+      </c>
+      <c r="FA23">
+        <v>0</v>
+      </c>
+      <c r="FD23">
+        <v>0</v>
+      </c>
+      <c r="FE23">
+        <v>0</v>
+      </c>
+      <c r="FF23">
+        <v>0</v>
+      </c>
+      <c r="FG23">
+        <v>0</v>
+      </c>
+      <c r="FH23">
+        <v>0</v>
+      </c>
+      <c r="FI23">
+        <v>0</v>
+      </c>
+      <c r="FJ23">
+        <v>0</v>
+      </c>
+      <c r="FK23">
+        <v>0</v>
+      </c>
+      <c r="FL23">
+        <v>0</v>
+      </c>
+      <c r="FM23">
+        <v>0</v>
+      </c>
+      <c r="FN23">
+        <v>0</v>
+      </c>
+      <c r="FO23" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP23">
+        <v>0</v>
+      </c>
+      <c r="FR23" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS23">
+        <v>0</v>
+      </c>
+      <c r="FU23">
+        <v>0</v>
+      </c>
+      <c r="FV23">
+        <v>0</v>
+      </c>
+      <c r="FW23">
+        <v>0</v>
+      </c>
+      <c r="FX23">
+        <v>0</v>
+      </c>
+      <c r="FY23">
+        <v>0</v>
+      </c>
+      <c r="FZ23">
+        <v>0</v>
+      </c>
+      <c r="GA23">
+        <v>0</v>
+      </c>
+      <c r="GB23">
+        <v>0</v>
+      </c>
+      <c r="GC23">
+        <v>0</v>
+      </c>
+      <c r="GD23">
+        <v>0</v>
+      </c>
+      <c r="GE23">
+        <v>0</v>
+      </c>
+      <c r="GF23">
+        <v>0</v>
+      </c>
+      <c r="GG23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:189">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24">
+        <v>20220401</v>
+      </c>
+      <c r="D24">
+        <v>99999999</v>
+      </c>
+      <c r="E24" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>364</v>
+      </c>
+      <c r="H24" t="s">
+        <v>371</v>
+      </c>
+      <c r="P24" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>343</v>
+      </c>
+      <c r="S24">
+        <v>47</v>
+      </c>
+      <c r="T24" t="s">
+        <v>279</v>
+      </c>
+      <c r="U24" t="s">
+        <v>279</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
+      </c>
+      <c r="AM24">
+        <v>0</v>
+      </c>
+      <c r="AN24">
+        <v>0</v>
+      </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>0</v>
+      </c>
+      <c r="AQ24">
+        <v>0</v>
+      </c>
+      <c r="AR24">
+        <v>0</v>
+      </c>
+      <c r="AS24">
+        <v>0</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
+      </c>
+      <c r="AU24">
+        <v>0</v>
+      </c>
+      <c r="AV24">
+        <v>0</v>
+      </c>
+      <c r="AW24">
+        <v>0</v>
+      </c>
+      <c r="AX24">
+        <v>0</v>
+      </c>
+      <c r="AY24">
+        <v>0</v>
+      </c>
+      <c r="AZ24">
+        <v>0</v>
+      </c>
+      <c r="BA24">
+        <v>0</v>
+      </c>
+      <c r="BB24">
+        <v>0</v>
+      </c>
+      <c r="BC24">
+        <v>0</v>
+      </c>
+      <c r="BD24">
+        <v>0</v>
+      </c>
+      <c r="BE24">
+        <v>0</v>
+      </c>
+      <c r="BF24">
+        <v>0</v>
+      </c>
+      <c r="BG24">
+        <v>0</v>
+      </c>
+      <c r="BH24">
+        <v>0</v>
+      </c>
+      <c r="BI24">
+        <v>0</v>
+      </c>
+      <c r="BJ24">
+        <v>0</v>
+      </c>
+      <c r="BK24">
+        <v>0</v>
+      </c>
+      <c r="BL24">
+        <v>0</v>
+      </c>
+      <c r="BM24">
+        <v>0</v>
+      </c>
+      <c r="BN24">
+        <v>0</v>
+      </c>
+      <c r="BO24">
+        <v>0</v>
+      </c>
+      <c r="BP24">
+        <v>0</v>
+      </c>
+      <c r="BQ24">
+        <v>0</v>
+      </c>
+      <c r="BR24">
+        <v>0</v>
+      </c>
+      <c r="BS24">
+        <v>0</v>
+      </c>
+      <c r="BT24">
+        <v>0</v>
+      </c>
+      <c r="BV24">
+        <v>0</v>
+      </c>
+      <c r="BW24">
+        <v>0</v>
+      </c>
+      <c r="BX24">
+        <v>0</v>
+      </c>
+      <c r="BY24">
+        <v>0</v>
+      </c>
+      <c r="BZ24">
+        <v>0</v>
+      </c>
+      <c r="CA24">
+        <v>0</v>
+      </c>
+      <c r="CB24">
+        <v>0</v>
+      </c>
+      <c r="CC24">
+        <v>0</v>
+      </c>
+      <c r="CD24">
+        <v>0</v>
+      </c>
+      <c r="CE24">
+        <v>0</v>
+      </c>
+      <c r="CF24">
+        <v>0</v>
+      </c>
+      <c r="CG24">
+        <v>0</v>
+      </c>
+      <c r="CT24">
+        <v>0</v>
+      </c>
+      <c r="CU24">
+        <v>0</v>
+      </c>
+      <c r="CV24">
+        <v>0</v>
+      </c>
+      <c r="CW24">
+        <v>0</v>
+      </c>
+      <c r="CX24">
+        <v>0</v>
+      </c>
+      <c r="CY24">
+        <v>4</v>
+      </c>
+      <c r="CZ24">
+        <v>0</v>
+      </c>
+      <c r="DA24">
+        <v>0</v>
+      </c>
+      <c r="DB24">
+        <v>0</v>
+      </c>
+      <c r="DC24">
+        <v>0</v>
+      </c>
+      <c r="DD24">
+        <v>0</v>
+      </c>
+      <c r="DE24">
+        <v>0</v>
+      </c>
+      <c r="DF24">
+        <v>0</v>
+      </c>
+      <c r="DG24">
+        <v>0</v>
+      </c>
+      <c r="DH24">
+        <v>0</v>
+      </c>
+      <c r="DJ24">
+        <v>0</v>
+      </c>
+      <c r="DK24">
+        <v>0</v>
+      </c>
+      <c r="DL24">
+        <v>0</v>
+      </c>
+      <c r="DM24">
+        <v>0</v>
+      </c>
+      <c r="DN24">
+        <v>0</v>
+      </c>
+      <c r="DP24">
+        <v>0</v>
+      </c>
+      <c r="DQ24">
+        <v>0</v>
+      </c>
+      <c r="DR24">
+        <v>0</v>
+      </c>
+      <c r="DS24">
+        <v>0</v>
+      </c>
+      <c r="DT24">
+        <v>0</v>
+      </c>
+      <c r="DU24">
+        <v>0</v>
+      </c>
+      <c r="DV24">
+        <v>0</v>
+      </c>
+      <c r="DW24">
+        <v>0</v>
+      </c>
+      <c r="DX24" t="s">
+        <v>449</v>
+      </c>
+      <c r="DY24" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ24">
+        <v>0</v>
+      </c>
+      <c r="EA24">
+        <v>0</v>
+      </c>
+      <c r="EB24">
+        <v>20220401</v>
+      </c>
+      <c r="EC24">
+        <v>99999999</v>
+      </c>
+      <c r="ED24">
+        <v>0</v>
+      </c>
+      <c r="EE24">
+        <v>0</v>
+      </c>
+      <c r="EF24">
+        <v>0</v>
+      </c>
+      <c r="EG24">
+        <v>0</v>
+      </c>
+      <c r="EH24">
+        <v>0</v>
+      </c>
+      <c r="EI24">
+        <v>0</v>
+      </c>
+      <c r="EJ24">
+        <v>0</v>
+      </c>
+      <c r="EK24">
+        <v>0</v>
+      </c>
+      <c r="EL24">
+        <v>0</v>
+      </c>
+      <c r="EM24">
+        <v>0</v>
+      </c>
+      <c r="EN24">
+        <v>0</v>
+      </c>
+      <c r="EO24">
+        <v>0</v>
+      </c>
+      <c r="EP24" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ24">
+        <v>0</v>
+      </c>
+      <c r="ER24">
+        <v>0</v>
+      </c>
+      <c r="ES24">
+        <v>0</v>
+      </c>
+      <c r="ET24">
+        <v>0</v>
+      </c>
+      <c r="EU24">
+        <v>0</v>
+      </c>
+      <c r="EV24">
+        <v>1</v>
+      </c>
+      <c r="EW24">
+        <v>0</v>
+      </c>
+      <c r="EX24">
+        <v>620001936</v>
+      </c>
+      <c r="EY24">
+        <v>0</v>
+      </c>
+      <c r="FA24">
+        <v>0</v>
+      </c>
+      <c r="FD24">
+        <v>0</v>
+      </c>
+      <c r="FE24">
+        <v>0</v>
+      </c>
+      <c r="FF24">
+        <v>0</v>
+      </c>
+      <c r="FG24">
+        <v>0</v>
+      </c>
+      <c r="FH24">
+        <v>0</v>
+      </c>
+      <c r="FI24">
+        <v>0</v>
+      </c>
+      <c r="FJ24">
+        <v>0</v>
+      </c>
+      <c r="FK24">
+        <v>0</v>
+      </c>
+      <c r="FL24">
+        <v>0</v>
+      </c>
+      <c r="FM24">
+        <v>0</v>
+      </c>
+      <c r="FN24">
+        <v>0</v>
+      </c>
+      <c r="FO24" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP24">
+        <v>0</v>
+      </c>
+      <c r="FR24" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS24">
+        <v>0</v>
+      </c>
+      <c r="FU24">
+        <v>0</v>
+      </c>
+      <c r="FV24">
+        <v>0</v>
+      </c>
+      <c r="FW24">
+        <v>0</v>
+      </c>
+      <c r="FX24">
+        <v>0</v>
+      </c>
+      <c r="FY24">
+        <v>0</v>
+      </c>
+      <c r="FZ24">
+        <v>0</v>
+      </c>
+      <c r="GA24">
+        <v>0</v>
+      </c>
+      <c r="GB24">
+        <v>0</v>
+      </c>
+      <c r="GC24">
+        <v>0</v>
+      </c>
+      <c r="GD24">
+        <v>0</v>
+      </c>
+      <c r="GE24">
+        <v>0</v>
+      </c>
+      <c r="GF24">
+        <v>0</v>
+      </c>
+      <c r="GG24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:189">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>454</v>
+      </c>
+      <c r="C25">
+        <v>20220401</v>
+      </c>
+      <c r="D25">
+        <v>99999999</v>
+      </c>
+      <c r="E25" t="s">
+        <v>230</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>364</v>
+      </c>
+      <c r="H25" t="s">
+        <v>371</v>
+      </c>
+      <c r="P25" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>343</v>
+      </c>
+      <c r="S25">
+        <v>47</v>
+      </c>
+      <c r="T25" t="s">
+        <v>279</v>
+      </c>
+      <c r="U25" t="s">
+        <v>279</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>0</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>0</v>
+      </c>
+      <c r="AM25">
+        <v>0</v>
+      </c>
+      <c r="AN25">
+        <v>0</v>
+      </c>
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+      <c r="AQ25">
+        <v>0</v>
+      </c>
+      <c r="AR25">
+        <v>0</v>
+      </c>
+      <c r="AS25">
+        <v>0</v>
+      </c>
+      <c r="AT25">
+        <v>0</v>
+      </c>
+      <c r="AU25">
+        <v>0</v>
+      </c>
+      <c r="AV25">
+        <v>0</v>
+      </c>
+      <c r="AW25">
+        <v>0</v>
+      </c>
+      <c r="AX25">
+        <v>0</v>
+      </c>
+      <c r="AY25">
+        <v>0</v>
+      </c>
+      <c r="AZ25">
+        <v>0</v>
+      </c>
+      <c r="BA25">
+        <v>0</v>
+      </c>
+      <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BC25">
+        <v>0</v>
+      </c>
+      <c r="BD25">
+        <v>0</v>
+      </c>
+      <c r="BE25">
+        <v>0</v>
+      </c>
+      <c r="BF25">
+        <v>0</v>
+      </c>
+      <c r="BG25">
+        <v>0</v>
+      </c>
+      <c r="BH25">
+        <v>0</v>
+      </c>
+      <c r="BI25">
+        <v>0</v>
+      </c>
+      <c r="BJ25">
+        <v>0</v>
+      </c>
+      <c r="BK25">
+        <v>0</v>
+      </c>
+      <c r="BL25">
+        <v>0</v>
+      </c>
+      <c r="BM25">
+        <v>0</v>
+      </c>
+      <c r="BN25">
+        <v>0</v>
+      </c>
+      <c r="BO25">
+        <v>0</v>
+      </c>
+      <c r="BP25">
+        <v>0</v>
+      </c>
+      <c r="BQ25">
+        <v>0</v>
+      </c>
+      <c r="BR25">
+        <v>0</v>
+      </c>
+      <c r="BS25">
+        <v>0</v>
+      </c>
+      <c r="BT25">
+        <v>0</v>
+      </c>
+      <c r="BV25">
+        <v>0</v>
+      </c>
+      <c r="BW25">
+        <v>0</v>
+      </c>
+      <c r="BX25">
+        <v>0</v>
+      </c>
+      <c r="BY25">
+        <v>0</v>
+      </c>
+      <c r="BZ25">
+        <v>0</v>
+      </c>
+      <c r="CA25">
+        <v>0</v>
+      </c>
+      <c r="CB25">
+        <v>0</v>
+      </c>
+      <c r="CC25">
+        <v>0</v>
+      </c>
+      <c r="CD25">
+        <v>0</v>
+      </c>
+      <c r="CE25">
+        <v>0</v>
+      </c>
+      <c r="CF25">
+        <v>0</v>
+      </c>
+      <c r="CG25">
+        <v>0</v>
+      </c>
+      <c r="CT25">
+        <v>0</v>
+      </c>
+      <c r="CU25">
+        <v>0</v>
+      </c>
+      <c r="CV25">
+        <v>0</v>
+      </c>
+      <c r="CW25">
+        <v>0</v>
+      </c>
+      <c r="CX25">
+        <v>0</v>
+      </c>
+      <c r="CY25">
+        <v>4</v>
+      </c>
+      <c r="CZ25">
+        <v>0</v>
+      </c>
+      <c r="DA25">
+        <v>0</v>
+      </c>
+      <c r="DB25">
+        <v>0</v>
+      </c>
+      <c r="DC25">
+        <v>0</v>
+      </c>
+      <c r="DD25">
+        <v>0</v>
+      </c>
+      <c r="DE25">
+        <v>0</v>
+      </c>
+      <c r="DF25">
+        <v>0</v>
+      </c>
+      <c r="DG25">
+        <v>0</v>
+      </c>
+      <c r="DH25">
+        <v>0</v>
+      </c>
+      <c r="DJ25">
+        <v>0</v>
+      </c>
+      <c r="DK25">
+        <v>0</v>
+      </c>
+      <c r="DL25">
+        <v>0</v>
+      </c>
+      <c r="DM25">
+        <v>0</v>
+      </c>
+      <c r="DN25">
+        <v>0</v>
+      </c>
+      <c r="DP25">
+        <v>0</v>
+      </c>
+      <c r="DQ25">
+        <v>0</v>
+      </c>
+      <c r="DR25">
+        <v>0</v>
+      </c>
+      <c r="DS25">
+        <v>0</v>
+      </c>
+      <c r="DT25">
+        <v>0</v>
+      </c>
+      <c r="DU25">
+        <v>0</v>
+      </c>
+      <c r="DV25">
+        <v>0</v>
+      </c>
+      <c r="DW25">
+        <v>0</v>
+      </c>
+      <c r="DX25" t="s">
+        <v>450</v>
+      </c>
+      <c r="DY25" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ25">
+        <v>0</v>
+      </c>
+      <c r="EA25">
+        <v>0</v>
+      </c>
+      <c r="EB25">
+        <v>20220401</v>
+      </c>
+      <c r="EC25">
+        <v>99999999</v>
+      </c>
+      <c r="ED25">
+        <v>0</v>
+      </c>
+      <c r="EE25">
+        <v>0</v>
+      </c>
+      <c r="EF25">
+        <v>0</v>
+      </c>
+      <c r="EG25">
+        <v>0</v>
+      </c>
+      <c r="EH25">
+        <v>0</v>
+      </c>
+      <c r="EI25">
+        <v>0</v>
+      </c>
+      <c r="EJ25">
+        <v>0</v>
+      </c>
+      <c r="EK25">
+        <v>0</v>
+      </c>
+      <c r="EL25">
+        <v>0</v>
+      </c>
+      <c r="EM25">
+        <v>0</v>
+      </c>
+      <c r="EN25">
+        <v>0</v>
+      </c>
+      <c r="EO25">
+        <v>0</v>
+      </c>
+      <c r="EP25" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ25">
+        <v>0</v>
+      </c>
+      <c r="ER25">
+        <v>0</v>
+      </c>
+      <c r="ES25">
+        <v>0</v>
+      </c>
+      <c r="ET25">
+        <v>0</v>
+      </c>
+      <c r="EU25">
+        <v>0</v>
+      </c>
+      <c r="EV25">
+        <v>1</v>
+      </c>
+      <c r="EW25">
+        <v>0</v>
+      </c>
+      <c r="EX25">
+        <v>620001936</v>
+      </c>
+      <c r="EY25">
+        <v>0</v>
+      </c>
+      <c r="FA25">
+        <v>0</v>
+      </c>
+      <c r="FD25">
+        <v>0</v>
+      </c>
+      <c r="FE25">
+        <v>0</v>
+      </c>
+      <c r="FF25">
+        <v>0</v>
+      </c>
+      <c r="FG25">
+        <v>0</v>
+      </c>
+      <c r="FH25">
+        <v>0</v>
+      </c>
+      <c r="FI25">
+        <v>0</v>
+      </c>
+      <c r="FJ25">
+        <v>0</v>
+      </c>
+      <c r="FK25">
+        <v>0</v>
+      </c>
+      <c r="FL25">
+        <v>0</v>
+      </c>
+      <c r="FM25">
+        <v>0</v>
+      </c>
+      <c r="FN25">
+        <v>0</v>
+      </c>
+      <c r="FO25" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP25">
+        <v>0</v>
+      </c>
+      <c r="FR25" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS25">
+        <v>0</v>
+      </c>
+      <c r="FU25">
+        <v>0</v>
+      </c>
+      <c r="FV25">
+        <v>0</v>
+      </c>
+      <c r="FW25">
+        <v>0</v>
+      </c>
+      <c r="FX25">
+        <v>0</v>
+      </c>
+      <c r="FY25">
+        <v>0</v>
+      </c>
+      <c r="FZ25">
+        <v>0</v>
+      </c>
+      <c r="GA25">
+        <v>0</v>
+      </c>
+      <c r="GB25">
+        <v>0</v>
+      </c>
+      <c r="GC25">
+        <v>0</v>
+      </c>
+      <c r="GD25">
+        <v>0</v>
+      </c>
+      <c r="GE25">
+        <v>0</v>
+      </c>
+      <c r="GF25">
+        <v>0</v>
+      </c>
+      <c r="GG25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:189">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>460</v>
+      </c>
+      <c r="C26">
+        <v>20220401</v>
+      </c>
+      <c r="D26">
+        <v>99999999</v>
+      </c>
+      <c r="E26" t="s">
+        <v>230</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>364</v>
+      </c>
+      <c r="H26" t="s">
+        <v>371</v>
+      </c>
+      <c r="P26" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>343</v>
+      </c>
+      <c r="S26">
+        <v>47</v>
+      </c>
+      <c r="T26" t="s">
+        <v>279</v>
+      </c>
+      <c r="U26" t="s">
+        <v>279</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>0</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+      <c r="AN26">
+        <v>0</v>
+      </c>
+      <c r="AO26">
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>0</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <v>0</v>
+      </c>
+      <c r="AU26">
+        <v>0</v>
+      </c>
+      <c r="AV26">
+        <v>0</v>
+      </c>
+      <c r="AW26">
+        <v>0</v>
+      </c>
+      <c r="AX26">
+        <v>0</v>
+      </c>
+      <c r="AY26">
+        <v>0</v>
+      </c>
+      <c r="AZ26">
+        <v>0</v>
+      </c>
+      <c r="BA26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
+      <c r="BF26">
+        <v>0</v>
+      </c>
+      <c r="BG26">
+        <v>0</v>
+      </c>
+      <c r="BH26">
+        <v>0</v>
+      </c>
+      <c r="BI26">
+        <v>0</v>
+      </c>
+      <c r="BJ26">
+        <v>0</v>
+      </c>
+      <c r="BK26">
+        <v>0</v>
+      </c>
+      <c r="BL26">
+        <v>0</v>
+      </c>
+      <c r="BM26">
+        <v>0</v>
+      </c>
+      <c r="BN26">
+        <v>0</v>
+      </c>
+      <c r="BO26">
+        <v>0</v>
+      </c>
+      <c r="BP26">
+        <v>0</v>
+      </c>
+      <c r="BQ26">
+        <v>0</v>
+      </c>
+      <c r="BR26">
+        <v>0</v>
+      </c>
+      <c r="BS26">
+        <v>0</v>
+      </c>
+      <c r="BT26">
+        <v>0</v>
+      </c>
+      <c r="BV26">
+        <v>0</v>
+      </c>
+      <c r="BW26">
+        <v>0</v>
+      </c>
+      <c r="BX26">
+        <v>0</v>
+      </c>
+      <c r="BY26">
+        <v>0</v>
+      </c>
+      <c r="BZ26">
+        <v>0</v>
+      </c>
+      <c r="CA26">
+        <v>0</v>
+      </c>
+      <c r="CB26">
+        <v>0</v>
+      </c>
+      <c r="CC26">
+        <v>0</v>
+      </c>
+      <c r="CD26">
+        <v>0</v>
+      </c>
+      <c r="CE26">
+        <v>0</v>
+      </c>
+      <c r="CF26">
+        <v>0</v>
+      </c>
+      <c r="CG26">
+        <v>0</v>
+      </c>
+      <c r="CT26">
+        <v>0</v>
+      </c>
+      <c r="CU26">
+        <v>0</v>
+      </c>
+      <c r="CV26">
+        <v>0</v>
+      </c>
+      <c r="CW26">
+        <v>0</v>
+      </c>
+      <c r="CX26">
+        <v>0</v>
+      </c>
+      <c r="CY26">
+        <v>4</v>
+      </c>
+      <c r="CZ26">
+        <v>0</v>
+      </c>
+      <c r="DA26">
+        <v>0</v>
+      </c>
+      <c r="DB26">
+        <v>0</v>
+      </c>
+      <c r="DC26">
+        <v>0</v>
+      </c>
+      <c r="DD26">
+        <v>0</v>
+      </c>
+      <c r="DE26">
+        <v>0</v>
+      </c>
+      <c r="DF26">
+        <v>0</v>
+      </c>
+      <c r="DG26">
+        <v>0</v>
+      </c>
+      <c r="DH26">
+        <v>0</v>
+      </c>
+      <c r="DJ26">
+        <v>0</v>
+      </c>
+      <c r="DK26">
+        <v>0</v>
+      </c>
+      <c r="DL26">
+        <v>0</v>
+      </c>
+      <c r="DM26">
+        <v>0</v>
+      </c>
+      <c r="DN26">
+        <v>0</v>
+      </c>
+      <c r="DP26">
+        <v>0</v>
+      </c>
+      <c r="DQ26">
+        <v>0</v>
+      </c>
+      <c r="DR26">
+        <v>0</v>
+      </c>
+      <c r="DS26">
+        <v>0</v>
+      </c>
+      <c r="DT26">
+        <v>0</v>
+      </c>
+      <c r="DU26">
+        <v>0</v>
+      </c>
+      <c r="DV26">
+        <v>0</v>
+      </c>
+      <c r="DW26">
+        <v>0</v>
+      </c>
+      <c r="DX26" t="s">
+        <v>457</v>
+      </c>
+      <c r="DY26" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ26">
+        <v>0</v>
+      </c>
+      <c r="EA26">
+        <v>0</v>
+      </c>
+      <c r="EB26">
+        <v>20220401</v>
+      </c>
+      <c r="EC26">
+        <v>99999999</v>
+      </c>
+      <c r="ED26">
+        <v>0</v>
+      </c>
+      <c r="EE26">
+        <v>0</v>
+      </c>
+      <c r="EF26">
+        <v>0</v>
+      </c>
+      <c r="EG26">
+        <v>0</v>
+      </c>
+      <c r="EH26">
+        <v>0</v>
+      </c>
+      <c r="EI26">
+        <v>0</v>
+      </c>
+      <c r="EJ26">
+        <v>0</v>
+      </c>
+      <c r="EK26">
+        <v>0</v>
+      </c>
+      <c r="EL26">
+        <v>0</v>
+      </c>
+      <c r="EM26">
+        <v>0</v>
+      </c>
+      <c r="EN26">
+        <v>0</v>
+      </c>
+      <c r="EO26">
+        <v>0</v>
+      </c>
+      <c r="EP26" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ26">
+        <v>0</v>
+      </c>
+      <c r="ER26">
+        <v>0</v>
+      </c>
+      <c r="ES26">
+        <v>0</v>
+      </c>
+      <c r="ET26">
+        <v>0</v>
+      </c>
+      <c r="EU26">
+        <v>0</v>
+      </c>
+      <c r="EV26">
+        <v>1</v>
+      </c>
+      <c r="EW26">
+        <v>0</v>
+      </c>
+      <c r="EX26">
+        <v>620001936</v>
+      </c>
+      <c r="EY26">
+        <v>0</v>
+      </c>
+      <c r="FA26">
+        <v>0</v>
+      </c>
+      <c r="FD26">
+        <v>0</v>
+      </c>
+      <c r="FE26">
+        <v>0</v>
+      </c>
+      <c r="FF26">
+        <v>0</v>
+      </c>
+      <c r="FG26">
+        <v>0</v>
+      </c>
+      <c r="FH26">
+        <v>0</v>
+      </c>
+      <c r="FI26">
+        <v>0</v>
+      </c>
+      <c r="FJ26">
+        <v>0</v>
+      </c>
+      <c r="FK26">
+        <v>0</v>
+      </c>
+      <c r="FL26">
+        <v>0</v>
+      </c>
+      <c r="FM26">
+        <v>0</v>
+      </c>
+      <c r="FN26">
+        <v>0</v>
+      </c>
+      <c r="FO26" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP26">
+        <v>0</v>
+      </c>
+      <c r="FR26" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS26">
+        <v>0</v>
+      </c>
+      <c r="FU26">
+        <v>0</v>
+      </c>
+      <c r="FV26">
+        <v>0</v>
+      </c>
+      <c r="FW26">
+        <v>0</v>
+      </c>
+      <c r="FX26">
+        <v>0</v>
+      </c>
+      <c r="FY26">
+        <v>0</v>
+      </c>
+      <c r="FZ26">
+        <v>0</v>
+      </c>
+      <c r="GA26">
+        <v>0</v>
+      </c>
+      <c r="GB26">
+        <v>0</v>
+      </c>
+      <c r="GC26">
+        <v>0</v>
+      </c>
+      <c r="GD26">
+        <v>0</v>
+      </c>
+      <c r="GE26">
+        <v>0</v>
+      </c>
+      <c r="GF26">
+        <v>0</v>
+      </c>
+      <c r="GG26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:189">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>461</v>
+      </c>
+      <c r="C27">
+        <v>20220401</v>
+      </c>
+      <c r="D27">
+        <v>99999999</v>
+      </c>
+      <c r="E27" t="s">
+        <v>230</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>364</v>
+      </c>
+      <c r="H27" t="s">
+        <v>371</v>
+      </c>
+      <c r="P27" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>343</v>
+      </c>
+      <c r="S27">
+        <v>47</v>
+      </c>
+      <c r="T27" t="s">
+        <v>279</v>
+      </c>
+      <c r="U27" t="s">
+        <v>279</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
+      <c r="AT27">
+        <v>0</v>
+      </c>
+      <c r="AU27">
+        <v>0</v>
+      </c>
+      <c r="AV27">
+        <v>0</v>
+      </c>
+      <c r="AW27">
+        <v>0</v>
+      </c>
+      <c r="AX27">
+        <v>0</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="AZ27">
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <v>0</v>
+      </c>
+      <c r="BF27">
+        <v>0</v>
+      </c>
+      <c r="BG27">
+        <v>0</v>
+      </c>
+      <c r="BH27">
+        <v>0</v>
+      </c>
+      <c r="BI27">
+        <v>0</v>
+      </c>
+      <c r="BJ27">
+        <v>0</v>
+      </c>
+      <c r="BK27">
+        <v>0</v>
+      </c>
+      <c r="BL27">
+        <v>0</v>
+      </c>
+      <c r="BM27">
+        <v>0</v>
+      </c>
+      <c r="BN27">
+        <v>0</v>
+      </c>
+      <c r="BO27">
+        <v>0</v>
+      </c>
+      <c r="BP27">
+        <v>0</v>
+      </c>
+      <c r="BQ27">
+        <v>0</v>
+      </c>
+      <c r="BR27">
+        <v>0</v>
+      </c>
+      <c r="BS27">
+        <v>0</v>
+      </c>
+      <c r="BT27">
+        <v>0</v>
+      </c>
+      <c r="BV27">
+        <v>0</v>
+      </c>
+      <c r="BW27">
+        <v>0</v>
+      </c>
+      <c r="BX27">
+        <v>0</v>
+      </c>
+      <c r="BY27">
+        <v>0</v>
+      </c>
+      <c r="BZ27">
+        <v>0</v>
+      </c>
+      <c r="CA27">
+        <v>0</v>
+      </c>
+      <c r="CB27">
+        <v>0</v>
+      </c>
+      <c r="CC27">
+        <v>0</v>
+      </c>
+      <c r="CD27">
+        <v>0</v>
+      </c>
+      <c r="CE27">
+        <v>0</v>
+      </c>
+      <c r="CF27">
+        <v>0</v>
+      </c>
+      <c r="CG27">
+        <v>0</v>
+      </c>
+      <c r="CT27">
+        <v>0</v>
+      </c>
+      <c r="CU27">
+        <v>0</v>
+      </c>
+      <c r="CV27">
+        <v>0</v>
+      </c>
+      <c r="CW27">
+        <v>0</v>
+      </c>
+      <c r="CX27">
+        <v>0</v>
+      </c>
+      <c r="CY27">
+        <v>4</v>
+      </c>
+      <c r="CZ27">
+        <v>0</v>
+      </c>
+      <c r="DA27">
+        <v>0</v>
+      </c>
+      <c r="DB27">
+        <v>0</v>
+      </c>
+      <c r="DC27">
+        <v>0</v>
+      </c>
+      <c r="DD27">
+        <v>0</v>
+      </c>
+      <c r="DE27">
+        <v>0</v>
+      </c>
+      <c r="DF27">
+        <v>0</v>
+      </c>
+      <c r="DG27">
+        <v>0</v>
+      </c>
+      <c r="DH27">
+        <v>0</v>
+      </c>
+      <c r="DJ27">
+        <v>0</v>
+      </c>
+      <c r="DK27">
+        <v>0</v>
+      </c>
+      <c r="DL27">
+        <v>0</v>
+      </c>
+      <c r="DM27">
+        <v>0</v>
+      </c>
+      <c r="DN27">
+        <v>0</v>
+      </c>
+      <c r="DP27">
+        <v>0</v>
+      </c>
+      <c r="DQ27">
+        <v>0</v>
+      </c>
+      <c r="DR27">
+        <v>0</v>
+      </c>
+      <c r="DS27">
+        <v>0</v>
+      </c>
+      <c r="DT27">
+        <v>0</v>
+      </c>
+      <c r="DU27">
+        <v>0</v>
+      </c>
+      <c r="DV27">
+        <v>0</v>
+      </c>
+      <c r="DW27">
+        <v>0</v>
+      </c>
+      <c r="DX27" t="s">
+        <v>459</v>
+      </c>
+      <c r="DY27" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ27">
+        <v>0</v>
+      </c>
+      <c r="EA27">
+        <v>0</v>
+      </c>
+      <c r="EB27">
+        <v>20220401</v>
+      </c>
+      <c r="EC27">
+        <v>99999999</v>
+      </c>
+      <c r="ED27">
+        <v>0</v>
+      </c>
+      <c r="EE27">
+        <v>0</v>
+      </c>
+      <c r="EF27">
+        <v>0</v>
+      </c>
+      <c r="EG27">
+        <v>0</v>
+      </c>
+      <c r="EH27">
+        <v>0</v>
+      </c>
+      <c r="EI27">
+        <v>0</v>
+      </c>
+      <c r="EJ27">
+        <v>0</v>
+      </c>
+      <c r="EK27">
+        <v>0</v>
+      </c>
+      <c r="EL27">
+        <v>0</v>
+      </c>
+      <c r="EM27">
+        <v>0</v>
+      </c>
+      <c r="EN27">
+        <v>0</v>
+      </c>
+      <c r="EO27">
+        <v>0</v>
+      </c>
+      <c r="EP27" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ27">
+        <v>0</v>
+      </c>
+      <c r="ER27">
+        <v>0</v>
+      </c>
+      <c r="ES27">
+        <v>0</v>
+      </c>
+      <c r="ET27">
+        <v>0</v>
+      </c>
+      <c r="EU27">
+        <v>0</v>
+      </c>
+      <c r="EV27">
+        <v>1</v>
+      </c>
+      <c r="EW27">
+        <v>0</v>
+      </c>
+      <c r="EX27">
+        <v>620001936</v>
+      </c>
+      <c r="EY27">
+        <v>0</v>
+      </c>
+      <c r="FA27">
+        <v>0</v>
+      </c>
+      <c r="FD27">
+        <v>0</v>
+      </c>
+      <c r="FE27">
+        <v>0</v>
+      </c>
+      <c r="FF27">
+        <v>0</v>
+      </c>
+      <c r="FG27">
+        <v>0</v>
+      </c>
+      <c r="FH27">
+        <v>0</v>
+      </c>
+      <c r="FI27">
+        <v>0</v>
+      </c>
+      <c r="FJ27">
+        <v>0</v>
+      </c>
+      <c r="FK27">
+        <v>0</v>
+      </c>
+      <c r="FL27">
+        <v>0</v>
+      </c>
+      <c r="FM27">
+        <v>0</v>
+      </c>
+      <c r="FN27">
+        <v>0</v>
+      </c>
+      <c r="FO27" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP27">
+        <v>0</v>
+      </c>
+      <c r="FR27" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS27">
+        <v>0</v>
+      </c>
+      <c r="FU27">
+        <v>0</v>
+      </c>
+      <c r="FV27">
+        <v>0</v>
+      </c>
+      <c r="FW27">
+        <v>0</v>
+      </c>
+      <c r="FX27">
+        <v>0</v>
+      </c>
+      <c r="FY27">
+        <v>0</v>
+      </c>
+      <c r="FZ27">
+        <v>0</v>
+      </c>
+      <c r="GA27">
+        <v>0</v>
+      </c>
+      <c r="GB27">
+        <v>0</v>
+      </c>
+      <c r="GC27">
+        <v>0</v>
+      </c>
+      <c r="GD27">
+        <v>0</v>
+      </c>
+      <c r="GE27">
+        <v>0</v>
+      </c>
+      <c r="GF27">
+        <v>0</v>
+      </c>
+      <c r="GG27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:189">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C28">
+        <v>20220401</v>
+      </c>
+      <c r="D28">
+        <v>99999999</v>
+      </c>
+      <c r="E28" t="s">
+        <v>230</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>364</v>
+      </c>
+      <c r="H28" t="s">
+        <v>371</v>
+      </c>
+      <c r="P28" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>343</v>
+      </c>
+      <c r="S28">
+        <v>47</v>
+      </c>
+      <c r="T28" t="s">
+        <v>279</v>
+      </c>
+      <c r="U28" t="s">
+        <v>279</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <v>0</v>
+      </c>
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AJ28">
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
+      </c>
+      <c r="AM28">
+        <v>0</v>
+      </c>
+      <c r="AN28">
+        <v>0</v>
+      </c>
+      <c r="AO28">
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <v>0</v>
+      </c>
+      <c r="AQ28">
+        <v>0</v>
+      </c>
+      <c r="AR28">
+        <v>0</v>
+      </c>
+      <c r="AS28">
+        <v>0</v>
+      </c>
+      <c r="AT28">
+        <v>0</v>
+      </c>
+      <c r="AU28">
+        <v>0</v>
+      </c>
+      <c r="AV28">
+        <v>0</v>
+      </c>
+      <c r="AW28">
+        <v>0</v>
+      </c>
+      <c r="AX28">
+        <v>0</v>
+      </c>
+      <c r="AY28">
+        <v>0</v>
+      </c>
+      <c r="AZ28">
+        <v>0</v>
+      </c>
+      <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>0</v>
+      </c>
+      <c r="BC28">
+        <v>0</v>
+      </c>
+      <c r="BD28">
+        <v>0</v>
+      </c>
+      <c r="BE28">
+        <v>0</v>
+      </c>
+      <c r="BF28">
+        <v>0</v>
+      </c>
+      <c r="BG28">
+        <v>0</v>
+      </c>
+      <c r="BH28">
+        <v>0</v>
+      </c>
+      <c r="BI28">
+        <v>0</v>
+      </c>
+      <c r="BJ28">
+        <v>0</v>
+      </c>
+      <c r="BK28">
+        <v>0</v>
+      </c>
+      <c r="BL28">
+        <v>0</v>
+      </c>
+      <c r="BM28">
+        <v>0</v>
+      </c>
+      <c r="BN28">
+        <v>0</v>
+      </c>
+      <c r="BO28">
+        <v>0</v>
+      </c>
+      <c r="BP28">
+        <v>0</v>
+      </c>
+      <c r="BQ28">
+        <v>0</v>
+      </c>
+      <c r="BR28">
+        <v>0</v>
+      </c>
+      <c r="BS28">
+        <v>0</v>
+      </c>
+      <c r="BT28">
+        <v>0</v>
+      </c>
+      <c r="BV28">
+        <v>0</v>
+      </c>
+      <c r="BW28">
+        <v>0</v>
+      </c>
+      <c r="BX28">
+        <v>0</v>
+      </c>
+      <c r="BY28">
+        <v>0</v>
+      </c>
+      <c r="BZ28">
+        <v>0</v>
+      </c>
+      <c r="CA28">
+        <v>0</v>
+      </c>
+      <c r="CB28">
+        <v>0</v>
+      </c>
+      <c r="CC28">
+        <v>0</v>
+      </c>
+      <c r="CD28">
+        <v>0</v>
+      </c>
+      <c r="CE28">
+        <v>0</v>
+      </c>
+      <c r="CF28">
+        <v>0</v>
+      </c>
+      <c r="CG28">
+        <v>0</v>
+      </c>
+      <c r="CT28">
+        <v>0</v>
+      </c>
+      <c r="CU28">
+        <v>0</v>
+      </c>
+      <c r="CV28">
+        <v>0</v>
+      </c>
+      <c r="CW28">
+        <v>0</v>
+      </c>
+      <c r="CX28">
+        <v>0</v>
+      </c>
+      <c r="CY28">
+        <v>4</v>
+      </c>
+      <c r="CZ28">
+        <v>0</v>
+      </c>
+      <c r="DA28">
+        <v>0</v>
+      </c>
+      <c r="DB28">
+        <v>0</v>
+      </c>
+      <c r="DC28">
+        <v>0</v>
+      </c>
+      <c r="DD28">
+        <v>0</v>
+      </c>
+      <c r="DE28">
+        <v>0</v>
+      </c>
+      <c r="DF28">
+        <v>0</v>
+      </c>
+      <c r="DG28">
+        <v>0</v>
+      </c>
+      <c r="DH28">
+        <v>0</v>
+      </c>
+      <c r="DJ28">
+        <v>0</v>
+      </c>
+      <c r="DK28">
+        <v>0</v>
+      </c>
+      <c r="DL28">
+        <v>0</v>
+      </c>
+      <c r="DM28">
+        <v>0</v>
+      </c>
+      <c r="DN28">
+        <v>0</v>
+      </c>
+      <c r="DP28">
+        <v>0</v>
+      </c>
+      <c r="DQ28">
+        <v>0</v>
+      </c>
+      <c r="DR28">
+        <v>0</v>
+      </c>
+      <c r="DS28">
+        <v>0</v>
+      </c>
+      <c r="DT28">
+        <v>0</v>
+      </c>
+      <c r="DU28">
+        <v>0</v>
+      </c>
+      <c r="DV28">
+        <v>0</v>
+      </c>
+      <c r="DW28">
+        <v>0</v>
+      </c>
+      <c r="DX28" t="s">
+        <v>469</v>
+      </c>
+      <c r="DY28" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ28">
+        <v>0</v>
+      </c>
+      <c r="EA28">
+        <v>0</v>
+      </c>
+      <c r="EB28">
+        <v>20220401</v>
+      </c>
+      <c r="EC28">
+        <v>99999999</v>
+      </c>
+      <c r="ED28">
+        <v>0</v>
+      </c>
+      <c r="EE28">
+        <v>0</v>
+      </c>
+      <c r="EF28">
+        <v>0</v>
+      </c>
+      <c r="EG28">
+        <v>0</v>
+      </c>
+      <c r="EH28">
+        <v>0</v>
+      </c>
+      <c r="EI28">
+        <v>0</v>
+      </c>
+      <c r="EJ28">
+        <v>0</v>
+      </c>
+      <c r="EK28">
+        <v>0</v>
+      </c>
+      <c r="EL28">
+        <v>0</v>
+      </c>
+      <c r="EM28">
+        <v>0</v>
+      </c>
+      <c r="EN28">
+        <v>0</v>
+      </c>
+      <c r="EO28">
+        <v>0</v>
+      </c>
+      <c r="EP28" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ28">
+        <v>0</v>
+      </c>
+      <c r="ER28">
+        <v>0</v>
+      </c>
+      <c r="ES28">
+        <v>0</v>
+      </c>
+      <c r="ET28">
+        <v>0</v>
+      </c>
+      <c r="EU28">
+        <v>0</v>
+      </c>
+      <c r="EV28">
+        <v>1</v>
+      </c>
+      <c r="EW28">
+        <v>0</v>
+      </c>
+      <c r="EX28">
+        <v>620001936</v>
+      </c>
+      <c r="EY28">
+        <v>0</v>
+      </c>
+      <c r="FA28">
+        <v>0</v>
+      </c>
+      <c r="FD28">
+        <v>0</v>
+      </c>
+      <c r="FE28">
+        <v>0</v>
+      </c>
+      <c r="FF28">
+        <v>0</v>
+      </c>
+      <c r="FG28">
+        <v>0</v>
+      </c>
+      <c r="FH28">
+        <v>0</v>
+      </c>
+      <c r="FI28">
+        <v>0</v>
+      </c>
+      <c r="FJ28">
+        <v>0</v>
+      </c>
+      <c r="FK28">
+        <v>0</v>
+      </c>
+      <c r="FL28">
+        <v>0</v>
+      </c>
+      <c r="FM28">
+        <v>0</v>
+      </c>
+      <c r="FN28">
+        <v>0</v>
+      </c>
+      <c r="FO28" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP28">
+        <v>0</v>
+      </c>
+      <c r="FR28" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS28">
+        <v>0</v>
+      </c>
+      <c r="FU28">
+        <v>0</v>
+      </c>
+      <c r="FV28">
+        <v>0</v>
+      </c>
+      <c r="FW28">
+        <v>0</v>
+      </c>
+      <c r="FX28">
+        <v>0</v>
+      </c>
+      <c r="FY28">
+        <v>0</v>
+      </c>
+      <c r="FZ28">
+        <v>0</v>
+      </c>
+      <c r="GA28">
+        <v>0</v>
+      </c>
+      <c r="GB28">
+        <v>0</v>
+      </c>
+      <c r="GC28">
+        <v>0</v>
+      </c>
+      <c r="GD28">
+        <v>0</v>
+      </c>
+      <c r="GE28">
+        <v>0</v>
+      </c>
+      <c r="GF28">
+        <v>0</v>
+      </c>
+      <c r="GG28">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69915254237288138" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15097,10 +18607,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15146,19 +18656,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>429</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>430</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -15169,7 +18682,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -15179,6 +18692,155 @@
       </c>
       <c r="F3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>450</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>432</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>432</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>459</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>429</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>429</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -15330,10 +18992,263 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>440</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>440</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>445</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>450</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>445</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>459</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>458</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A3:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15350,29 +19265,29 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -15380,12 +19295,144 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15506,7 +19553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
@@ -15652,7 +19699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -15683,41 +19730,6 @@
       </c>
       <c r="B2" t="s">
         <v>391</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B2" t="s">
-        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -16025,6 +20037,41 @@
       </c>
       <c r="H12" t="s">
         <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UT cover CheckDuplicatedComponent RealtimeCheckerFinder
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="961" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="484">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1461,13 +1461,52 @@
   </si>
   <si>
     <t>UT2708</t>
+  </si>
+  <si>
+    <t>UT2709</t>
+  </si>
+  <si>
+    <t>UT271016</t>
+  </si>
+  <si>
+    <t>UT2710</t>
+  </si>
+  <si>
+    <t>UT271017</t>
+  </si>
+  <si>
+    <t>UT271018</t>
+  </si>
+  <si>
+    <t>UT271019</t>
+  </si>
+  <si>
+    <t>UT2711</t>
+  </si>
+  <si>
+    <t>UT2712</t>
+  </si>
+  <si>
+    <t>UT271020</t>
+  </si>
+  <si>
+    <t>UT2713</t>
+  </si>
+  <si>
+    <t>UT271021</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>UT2714</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1618,6 +1657,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1962,12 +2009,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="47" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4408,10 +4457,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG28"/>
+  <dimension ref="A1:GG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="DM1" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="DW28" sqref="DW28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -17917,6 +17966,2916 @@
         <v>0</v>
       </c>
       <c r="GG28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:189">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>471</v>
+      </c>
+      <c r="C29">
+        <v>20220401</v>
+      </c>
+      <c r="D29">
+        <v>99999999</v>
+      </c>
+      <c r="E29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>364</v>
+      </c>
+      <c r="H29" t="s">
+        <v>371</v>
+      </c>
+      <c r="P29" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>343</v>
+      </c>
+      <c r="S29">
+        <v>47</v>
+      </c>
+      <c r="T29" t="s">
+        <v>279</v>
+      </c>
+      <c r="U29" t="s">
+        <v>279</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <v>0</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
+      </c>
+      <c r="AM29">
+        <v>0</v>
+      </c>
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <v>0</v>
+      </c>
+      <c r="AQ29">
+        <v>0</v>
+      </c>
+      <c r="AR29">
+        <v>0</v>
+      </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
+      <c r="AT29">
+        <v>0</v>
+      </c>
+      <c r="AU29">
+        <v>0</v>
+      </c>
+      <c r="AV29">
+        <v>0</v>
+      </c>
+      <c r="AW29">
+        <v>0</v>
+      </c>
+      <c r="AX29">
+        <v>0</v>
+      </c>
+      <c r="AY29">
+        <v>0</v>
+      </c>
+      <c r="AZ29">
+        <v>0</v>
+      </c>
+      <c r="BA29">
+        <v>0</v>
+      </c>
+      <c r="BB29">
+        <v>0</v>
+      </c>
+      <c r="BC29">
+        <v>0</v>
+      </c>
+      <c r="BD29">
+        <v>0</v>
+      </c>
+      <c r="BE29">
+        <v>0</v>
+      </c>
+      <c r="BF29">
+        <v>0</v>
+      </c>
+      <c r="BG29">
+        <v>0</v>
+      </c>
+      <c r="BH29">
+        <v>0</v>
+      </c>
+      <c r="BI29">
+        <v>0</v>
+      </c>
+      <c r="BJ29">
+        <v>0</v>
+      </c>
+      <c r="BK29">
+        <v>0</v>
+      </c>
+      <c r="BL29">
+        <v>0</v>
+      </c>
+      <c r="BM29">
+        <v>0</v>
+      </c>
+      <c r="BN29">
+        <v>0</v>
+      </c>
+      <c r="BO29">
+        <v>0</v>
+      </c>
+      <c r="BP29">
+        <v>0</v>
+      </c>
+      <c r="BQ29">
+        <v>0</v>
+      </c>
+      <c r="BR29">
+        <v>0</v>
+      </c>
+      <c r="BS29">
+        <v>0</v>
+      </c>
+      <c r="BT29">
+        <v>0</v>
+      </c>
+      <c r="BV29">
+        <v>0</v>
+      </c>
+      <c r="BW29">
+        <v>0</v>
+      </c>
+      <c r="BX29">
+        <v>0</v>
+      </c>
+      <c r="BY29">
+        <v>0</v>
+      </c>
+      <c r="BZ29">
+        <v>0</v>
+      </c>
+      <c r="CA29">
+        <v>0</v>
+      </c>
+      <c r="CB29">
+        <v>0</v>
+      </c>
+      <c r="CC29">
+        <v>0</v>
+      </c>
+      <c r="CD29">
+        <v>0</v>
+      </c>
+      <c r="CE29">
+        <v>0</v>
+      </c>
+      <c r="CF29">
+        <v>0</v>
+      </c>
+      <c r="CG29">
+        <v>0</v>
+      </c>
+      <c r="CT29">
+        <v>0</v>
+      </c>
+      <c r="CU29">
+        <v>0</v>
+      </c>
+      <c r="CV29">
+        <v>0</v>
+      </c>
+      <c r="CW29">
+        <v>0</v>
+      </c>
+      <c r="CX29">
+        <v>0</v>
+      </c>
+      <c r="CY29">
+        <v>4</v>
+      </c>
+      <c r="CZ29">
+        <v>0</v>
+      </c>
+      <c r="DA29">
+        <v>0</v>
+      </c>
+      <c r="DB29">
+        <v>0</v>
+      </c>
+      <c r="DC29">
+        <v>0</v>
+      </c>
+      <c r="DD29">
+        <v>0</v>
+      </c>
+      <c r="DE29">
+        <v>0</v>
+      </c>
+      <c r="DF29">
+        <v>0</v>
+      </c>
+      <c r="DG29">
+        <v>0</v>
+      </c>
+      <c r="DH29">
+        <v>0</v>
+      </c>
+      <c r="DJ29">
+        <v>0</v>
+      </c>
+      <c r="DK29">
+        <v>0</v>
+      </c>
+      <c r="DL29">
+        <v>0</v>
+      </c>
+      <c r="DM29">
+        <v>0</v>
+      </c>
+      <c r="DN29">
+        <v>0</v>
+      </c>
+      <c r="DP29">
+        <v>0</v>
+      </c>
+      <c r="DQ29">
+        <v>0</v>
+      </c>
+      <c r="DR29">
+        <v>0</v>
+      </c>
+      <c r="DS29">
+        <v>0</v>
+      </c>
+      <c r="DT29">
+        <v>0</v>
+      </c>
+      <c r="DU29">
+        <v>0</v>
+      </c>
+      <c r="DV29">
+        <v>0</v>
+      </c>
+      <c r="DW29">
+        <v>0</v>
+      </c>
+      <c r="DX29" t="s">
+        <v>472</v>
+      </c>
+      <c r="DY29" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ29">
+        <v>0</v>
+      </c>
+      <c r="EA29">
+        <v>0</v>
+      </c>
+      <c r="EB29">
+        <v>20220401</v>
+      </c>
+      <c r="EC29">
+        <v>99999999</v>
+      </c>
+      <c r="ED29">
+        <v>0</v>
+      </c>
+      <c r="EE29">
+        <v>0</v>
+      </c>
+      <c r="EF29">
+        <v>0</v>
+      </c>
+      <c r="EG29">
+        <v>0</v>
+      </c>
+      <c r="EH29">
+        <v>0</v>
+      </c>
+      <c r="EI29">
+        <v>0</v>
+      </c>
+      <c r="EJ29">
+        <v>0</v>
+      </c>
+      <c r="EK29">
+        <v>0</v>
+      </c>
+      <c r="EL29">
+        <v>0</v>
+      </c>
+      <c r="EM29">
+        <v>0</v>
+      </c>
+      <c r="EN29">
+        <v>0</v>
+      </c>
+      <c r="EO29">
+        <v>0</v>
+      </c>
+      <c r="EP29" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ29">
+        <v>0</v>
+      </c>
+      <c r="ER29">
+        <v>0</v>
+      </c>
+      <c r="ES29">
+        <v>0</v>
+      </c>
+      <c r="ET29">
+        <v>0</v>
+      </c>
+      <c r="EU29">
+        <v>0</v>
+      </c>
+      <c r="EV29">
+        <v>1</v>
+      </c>
+      <c r="EW29">
+        <v>0</v>
+      </c>
+      <c r="EX29">
+        <v>620001936</v>
+      </c>
+      <c r="EY29">
+        <v>0</v>
+      </c>
+      <c r="FA29">
+        <v>0</v>
+      </c>
+      <c r="FD29">
+        <v>0</v>
+      </c>
+      <c r="FE29">
+        <v>0</v>
+      </c>
+      <c r="FF29">
+        <v>0</v>
+      </c>
+      <c r="FG29">
+        <v>0</v>
+      </c>
+      <c r="FH29">
+        <v>0</v>
+      </c>
+      <c r="FI29">
+        <v>0</v>
+      </c>
+      <c r="FJ29">
+        <v>0</v>
+      </c>
+      <c r="FK29">
+        <v>0</v>
+      </c>
+      <c r="FL29">
+        <v>0</v>
+      </c>
+      <c r="FM29">
+        <v>0</v>
+      </c>
+      <c r="FN29">
+        <v>0</v>
+      </c>
+      <c r="FO29" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP29">
+        <v>0</v>
+      </c>
+      <c r="FR29" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS29">
+        <v>0</v>
+      </c>
+      <c r="FU29">
+        <v>0</v>
+      </c>
+      <c r="FV29">
+        <v>0</v>
+      </c>
+      <c r="FW29">
+        <v>0</v>
+      </c>
+      <c r="FX29">
+        <v>0</v>
+      </c>
+      <c r="FY29">
+        <v>0</v>
+      </c>
+      <c r="FZ29">
+        <v>0</v>
+      </c>
+      <c r="GA29">
+        <v>0</v>
+      </c>
+      <c r="GB29">
+        <v>0</v>
+      </c>
+      <c r="GC29">
+        <v>0</v>
+      </c>
+      <c r="GD29">
+        <v>0</v>
+      </c>
+      <c r="GE29">
+        <v>0</v>
+      </c>
+      <c r="GF29">
+        <v>0</v>
+      </c>
+      <c r="GG29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:189" s="5" customFormat="1">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="C30" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D30" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" s="5">
+        <v>30</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>1</v>
+      </c>
+      <c r="R30" s="5">
+        <v>343</v>
+      </c>
+      <c r="S30" s="5">
+        <v>47</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W30" s="5">
+        <v>0</v>
+      </c>
+      <c r="X30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY30" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX30" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="DY30" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB30" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC30" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP30" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER30" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES30" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV30" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX30" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO30" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR30" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY30" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:189">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>477</v>
+      </c>
+      <c r="C31">
+        <v>20220401</v>
+      </c>
+      <c r="D31">
+        <v>99999999</v>
+      </c>
+      <c r="E31" t="s">
+        <v>230</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>364</v>
+      </c>
+      <c r="H31" t="s">
+        <v>371</v>
+      </c>
+      <c r="P31" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>343</v>
+      </c>
+      <c r="S31">
+        <v>47</v>
+      </c>
+      <c r="T31" t="s">
+        <v>279</v>
+      </c>
+      <c r="U31" t="s">
+        <v>279</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <v>0</v>
+      </c>
+      <c r="AO31">
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31">
+        <v>0</v>
+      </c>
+      <c r="AS31">
+        <v>0</v>
+      </c>
+      <c r="AT31">
+        <v>0</v>
+      </c>
+      <c r="AU31">
+        <v>0</v>
+      </c>
+      <c r="AV31">
+        <v>0</v>
+      </c>
+      <c r="AW31">
+        <v>0</v>
+      </c>
+      <c r="AX31">
+        <v>0</v>
+      </c>
+      <c r="AY31">
+        <v>0</v>
+      </c>
+      <c r="AZ31">
+        <v>0</v>
+      </c>
+      <c r="BA31">
+        <v>0</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31">
+        <v>0</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+      <c r="BE31">
+        <v>0</v>
+      </c>
+      <c r="BF31">
+        <v>0</v>
+      </c>
+      <c r="BG31">
+        <v>0</v>
+      </c>
+      <c r="BH31">
+        <v>0</v>
+      </c>
+      <c r="BI31">
+        <v>0</v>
+      </c>
+      <c r="BJ31">
+        <v>0</v>
+      </c>
+      <c r="BK31">
+        <v>0</v>
+      </c>
+      <c r="BL31">
+        <v>0</v>
+      </c>
+      <c r="BM31">
+        <v>0</v>
+      </c>
+      <c r="BN31">
+        <v>0</v>
+      </c>
+      <c r="BO31">
+        <v>0</v>
+      </c>
+      <c r="BP31">
+        <v>0</v>
+      </c>
+      <c r="BQ31">
+        <v>0</v>
+      </c>
+      <c r="BR31">
+        <v>0</v>
+      </c>
+      <c r="BS31">
+        <v>0</v>
+      </c>
+      <c r="BT31">
+        <v>0</v>
+      </c>
+      <c r="BV31">
+        <v>0</v>
+      </c>
+      <c r="BW31">
+        <v>0</v>
+      </c>
+      <c r="BX31">
+        <v>0</v>
+      </c>
+      <c r="BY31">
+        <v>0</v>
+      </c>
+      <c r="BZ31">
+        <v>0</v>
+      </c>
+      <c r="CA31">
+        <v>0</v>
+      </c>
+      <c r="CB31">
+        <v>0</v>
+      </c>
+      <c r="CC31">
+        <v>0</v>
+      </c>
+      <c r="CD31">
+        <v>0</v>
+      </c>
+      <c r="CE31">
+        <v>0</v>
+      </c>
+      <c r="CF31">
+        <v>0</v>
+      </c>
+      <c r="CG31">
+        <v>0</v>
+      </c>
+      <c r="CT31">
+        <v>0</v>
+      </c>
+      <c r="CU31">
+        <v>0</v>
+      </c>
+      <c r="CV31">
+        <v>0</v>
+      </c>
+      <c r="CW31">
+        <v>0</v>
+      </c>
+      <c r="CX31">
+        <v>0</v>
+      </c>
+      <c r="CY31">
+        <v>4</v>
+      </c>
+      <c r="CZ31">
+        <v>0</v>
+      </c>
+      <c r="DA31">
+        <v>0</v>
+      </c>
+      <c r="DB31">
+        <v>0</v>
+      </c>
+      <c r="DC31">
+        <v>0</v>
+      </c>
+      <c r="DD31">
+        <v>0</v>
+      </c>
+      <c r="DE31">
+        <v>0</v>
+      </c>
+      <c r="DF31">
+        <v>0</v>
+      </c>
+      <c r="DG31">
+        <v>0</v>
+      </c>
+      <c r="DH31">
+        <v>0</v>
+      </c>
+      <c r="DJ31">
+        <v>0</v>
+      </c>
+      <c r="DK31">
+        <v>0</v>
+      </c>
+      <c r="DL31">
+        <v>0</v>
+      </c>
+      <c r="DM31">
+        <v>0</v>
+      </c>
+      <c r="DN31">
+        <v>0</v>
+      </c>
+      <c r="DP31">
+        <v>0</v>
+      </c>
+      <c r="DQ31">
+        <v>0</v>
+      </c>
+      <c r="DR31">
+        <v>0</v>
+      </c>
+      <c r="DS31">
+        <v>0</v>
+      </c>
+      <c r="DT31">
+        <v>0</v>
+      </c>
+      <c r="DU31">
+        <v>0</v>
+      </c>
+      <c r="DV31">
+        <v>0</v>
+      </c>
+      <c r="DW31">
+        <v>0</v>
+      </c>
+      <c r="DX31" t="s">
+        <v>475</v>
+      </c>
+      <c r="DY31" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ31">
+        <v>0</v>
+      </c>
+      <c r="EA31">
+        <v>0</v>
+      </c>
+      <c r="EB31">
+        <v>20220401</v>
+      </c>
+      <c r="EC31">
+        <v>99999999</v>
+      </c>
+      <c r="ED31">
+        <v>0</v>
+      </c>
+      <c r="EE31">
+        <v>0</v>
+      </c>
+      <c r="EF31">
+        <v>0</v>
+      </c>
+      <c r="EG31">
+        <v>0</v>
+      </c>
+      <c r="EH31">
+        <v>0</v>
+      </c>
+      <c r="EI31">
+        <v>0</v>
+      </c>
+      <c r="EJ31">
+        <v>0</v>
+      </c>
+      <c r="EK31">
+        <v>0</v>
+      </c>
+      <c r="EL31">
+        <v>0</v>
+      </c>
+      <c r="EM31">
+        <v>0</v>
+      </c>
+      <c r="EN31">
+        <v>0</v>
+      </c>
+      <c r="EO31">
+        <v>0</v>
+      </c>
+      <c r="EP31" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ31">
+        <v>0</v>
+      </c>
+      <c r="ER31">
+        <v>0</v>
+      </c>
+      <c r="ES31">
+        <v>0</v>
+      </c>
+      <c r="ET31">
+        <v>0</v>
+      </c>
+      <c r="EU31">
+        <v>0</v>
+      </c>
+      <c r="EV31">
+        <v>1</v>
+      </c>
+      <c r="EW31">
+        <v>0</v>
+      </c>
+      <c r="EX31">
+        <v>620001936</v>
+      </c>
+      <c r="EY31">
+        <v>0</v>
+      </c>
+      <c r="FA31">
+        <v>0</v>
+      </c>
+      <c r="FD31">
+        <v>0</v>
+      </c>
+      <c r="FE31">
+        <v>0</v>
+      </c>
+      <c r="FF31">
+        <v>0</v>
+      </c>
+      <c r="FG31">
+        <v>0</v>
+      </c>
+      <c r="FH31">
+        <v>0</v>
+      </c>
+      <c r="FI31">
+        <v>0</v>
+      </c>
+      <c r="FJ31">
+        <v>0</v>
+      </c>
+      <c r="FK31">
+        <v>0</v>
+      </c>
+      <c r="FL31">
+        <v>0</v>
+      </c>
+      <c r="FM31">
+        <v>0</v>
+      </c>
+      <c r="FN31">
+        <v>0</v>
+      </c>
+      <c r="FO31" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FP31">
+        <v>0</v>
+      </c>
+      <c r="FR31" s="1">
+        <v>44627</v>
+      </c>
+      <c r="FS31">
+        <v>0</v>
+      </c>
+      <c r="FU31">
+        <v>0</v>
+      </c>
+      <c r="FV31">
+        <v>0</v>
+      </c>
+      <c r="FW31">
+        <v>0</v>
+      </c>
+      <c r="FX31">
+        <v>0</v>
+      </c>
+      <c r="FY31">
+        <v>0</v>
+      </c>
+      <c r="FZ31">
+        <v>0</v>
+      </c>
+      <c r="GA31">
+        <v>0</v>
+      </c>
+      <c r="GB31">
+        <v>0</v>
+      </c>
+      <c r="GC31">
+        <v>0</v>
+      </c>
+      <c r="GD31">
+        <v>0</v>
+      </c>
+      <c r="GE31">
+        <v>0</v>
+      </c>
+      <c r="GF31">
+        <v>0</v>
+      </c>
+      <c r="GG31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:189" s="5" customFormat="1">
+      <c r="A32" s="5">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C32" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D32" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F32" s="5">
+        <v>30</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>1</v>
+      </c>
+      <c r="R32" s="5">
+        <v>343</v>
+      </c>
+      <c r="S32" s="5">
+        <v>47</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W32" s="5">
+        <v>0</v>
+      </c>
+      <c r="X32" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY32" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY32" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX32" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY32" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX32" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="DY32" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB32" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC32" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP32" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER32" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES32" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV32" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX32" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO32" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR32" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY32" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF32" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:189" s="5" customFormat="1">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C33" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D33" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F33" s="5">
+        <v>30</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>1</v>
+      </c>
+      <c r="R33" s="5">
+        <v>343</v>
+      </c>
+      <c r="S33" s="5">
+        <v>47</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W33" s="5">
+        <v>0</v>
+      </c>
+      <c r="X33" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY33" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY33" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX33" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY33" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX33" t="s">
+        <v>479</v>
+      </c>
+      <c r="DY33" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB33" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC33" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP33" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER33" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES33" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV33" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX33" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO33" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR33" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY33" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF33" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:189" s="5" customFormat="1">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C34" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D34" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F34" s="5">
+        <v>30</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>1</v>
+      </c>
+      <c r="R34" s="5">
+        <v>343</v>
+      </c>
+      <c r="S34" s="5">
+        <v>47</v>
+      </c>
+      <c r="T34" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W34" s="5">
+        <v>0</v>
+      </c>
+      <c r="X34" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY34" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY34" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX34" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY34" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX34" t="s">
+        <v>481</v>
+      </c>
+      <c r="DY34" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB34" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC34" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP34" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER34" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES34" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV34" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX34" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO34" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR34" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY34" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF34" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG34" s="5">
         <v>0</v>
       </c>
     </row>
@@ -18607,10 +21566,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -18840,6 +21799,126 @@
         <v>0</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>474</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>429</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>475</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>429</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>429</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>479</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>429</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>481</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="C16" t="s">
+        <v>429</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UT cover CheckContraindicationForHistoryDisease RealtimeCheckerFinder
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="13" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -4460,7 +4460,7 @@
   <dimension ref="A1:GG34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21059,7 +21059,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21568,7 +21568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -21931,8 +21931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="A15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22821,7 +22821,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Cover UT CheckKinkiTain RealtimeCheckerFinder
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="22" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="493">
   <si>
     <t>HP_ID</t>
   </si>
@@ -4486,8 +4486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG38"/>
   <sheetViews>
-    <sheetView topLeftCell="DH1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="DV28" sqref="DV28"/>
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22857,7 +22857,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -24489,8 +24489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25966,9 +25966,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -26123,6 +26123,50 @@
         <v>349</v>
       </c>
     </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>483</v>
+      </c>
+      <c r="F4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>99999999</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>45104.430274398146</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>349</v>
+      </c>
+      <c r="N4" s="1">
+        <v>45104.430274398146</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>349</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cover UT CheckKinkiOTC RealtimeCheckerFinder
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="23" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="494">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1527,6 +1527,9 @@
   </si>
   <si>
     <t>UT27102</t>
+  </si>
+  <si>
+    <t>UT2719</t>
   </si>
 </sst>
 </file>
@@ -4484,16 +4487,17 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG38"/>
+  <dimension ref="A1:GG39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="128" max="128" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="10" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22843,6 +22847,491 @@
         <v>0</v>
       </c>
       <c r="GG38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:189" s="5" customFormat="1">
+      <c r="A39" s="5">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C39" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D39" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" s="5">
+        <v>30</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1</v>
+      </c>
+      <c r="R39" s="5">
+        <v>343</v>
+      </c>
+      <c r="S39" s="5">
+        <v>47</v>
+      </c>
+      <c r="T39" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U39" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W39" s="5">
+        <v>0</v>
+      </c>
+      <c r="X39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY39" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX39" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY39" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX39">
+        <v>9999999</v>
+      </c>
+      <c r="DY39" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB39" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC39" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP39" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER39" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES39" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV39" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX39" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO39" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR39" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY39" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG39" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24487,10 +24976,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -24644,6 +25133,40 @@
       </c>
       <c r="G7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>492</v>
+      </c>
+      <c r="B8">
+        <v>9999999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>9999999</v>
+      </c>
+      <c r="B9">
+        <v>9999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" t="s">
+        <v>387</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -25968,7 +26491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cover UT CheckDosage RealtimeCheckerFinder
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="22" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="25" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,18 @@
     <sheet name="M56_DRUG_CLASS" sheetId="30" r:id="rId25"/>
     <sheet name="M56_EX_ANALOGUE" sheetId="31" r:id="rId26"/>
     <sheet name="M01_KINKI" sheetId="14" r:id="rId27"/>
-    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId28"/>
-    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId29"/>
-    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId30"/>
+    <sheet name="DOSAGE_MST" sheetId="34" r:id="rId28"/>
+    <sheet name="M46_DOSAGE_DRUG" sheetId="35" r:id="rId29"/>
+    <sheet name="PT_SUPPLE" sheetId="15" r:id="rId30"/>
+    <sheet name="M41_SUPPLE_INDEXDEF" sheetId="16" r:id="rId31"/>
+    <sheet name="M41_SUPPLE_INDEXCODE" sheetId="17" r:id="rId32"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="513">
   <si>
     <t>HP_ID</t>
   </si>
@@ -1530,6 +1532,63 @@
   </si>
   <si>
     <t>UT2719</t>
+  </si>
+  <si>
+    <t>ONCE_MIN</t>
+  </si>
+  <si>
+    <t>ONCE_MAX</t>
+  </si>
+  <si>
+    <t>ONCE_LIMIT</t>
+  </si>
+  <si>
+    <t>ONCE_UNIT</t>
+  </si>
+  <si>
+    <t>DAY_MIN</t>
+  </si>
+  <si>
+    <t>DAY_MAX</t>
+  </si>
+  <si>
+    <t>DAY_LIMIT</t>
+  </si>
+  <si>
+    <t>DAY_UNIT</t>
+  </si>
+  <si>
+    <t>6163OONS12</t>
+  </si>
+  <si>
+    <t>UT2720</t>
+  </si>
+  <si>
+    <t>UT271026</t>
+  </si>
+  <si>
+    <t>DOEI_CD</t>
+  </si>
+  <si>
+    <t>KIKAKU_UNIT</t>
+  </si>
+  <si>
+    <t>YAKKA_UNIT</t>
+  </si>
+  <si>
+    <t>RIKIKA_RATE</t>
+  </si>
+  <si>
+    <t>RIKIKA_UNIT</t>
+  </si>
+  <si>
+    <t>YOUKAIEKI_CD</t>
+  </si>
+  <si>
+    <t>ï¼‘ï½ï¼¬</t>
+  </si>
+  <si>
+    <t>mL</t>
   </si>
 </sst>
 </file>
@@ -4487,10 +4546,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG39"/>
+  <dimension ref="A1:GG40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23332,6 +23391,491 @@
         <v>0</v>
       </c>
       <c r="GG39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:189" s="5" customFormat="1">
+      <c r="A40" s="5">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="C40" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="D40" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F40" s="5">
+        <v>30</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>1</v>
+      </c>
+      <c r="R40" s="5">
+        <v>343</v>
+      </c>
+      <c r="S40" s="5">
+        <v>47</v>
+      </c>
+      <c r="T40" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="U40" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="W40" s="5">
+        <v>0</v>
+      </c>
+      <c r="X40" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY40" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX40" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY40" s="5">
+        <v>4</v>
+      </c>
+      <c r="CZ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX40" t="s">
+        <v>504</v>
+      </c>
+      <c r="DY40" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="DZ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB40" s="5">
+        <v>20220401</v>
+      </c>
+      <c r="EC40" s="5">
+        <v>99999999</v>
+      </c>
+      <c r="ED40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP40" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="EQ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER40" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES40" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV40" s="5">
+        <v>1</v>
+      </c>
+      <c r="EW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX40" s="5">
+        <v>620001936</v>
+      </c>
+      <c r="EY40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO40" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FP40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR40" s="6">
+        <v>44627</v>
+      </c>
+      <c r="FS40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY40" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GD40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GE40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GF40" s="5">
+        <v>0</v>
+      </c>
+      <c r="GG40" s="5">
         <v>0</v>
       </c>
     </row>
@@ -24978,8 +25522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25192,6 +25736,525 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>494</v>
+      </c>
+      <c r="F1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" t="s">
+        <v>496</v>
+      </c>
+      <c r="H1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I1" t="s">
+        <v>498</v>
+      </c>
+      <c r="J1" t="s">
+        <v>499</v>
+      </c>
+      <c r="K1" t="s">
+        <v>500</v>
+      </c>
+      <c r="L1" t="s">
+        <v>501</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2">
+        <v>9999999</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>999</v>
+      </c>
+      <c r="G2">
+        <v>999</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>41558.86886574074</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>41558.86886574074</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E1" t="s">
+        <v>507</v>
+      </c>
+      <c r="F1" t="s">
+        <v>508</v>
+      </c>
+      <c r="G1" t="s">
+        <v>509</v>
+      </c>
+      <c r="H1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B2">
+        <v>11127000</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>267</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>267</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
@@ -25375,7 +26438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -25413,314 +26476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" t="s">
-        <v>250</v>
-      </c>
-      <c r="D1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>267</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>267</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>300</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>267</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>267</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>302</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>267</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>267</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>299</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>267</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>412</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>267</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
merge dev to SMAR-6376
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="23" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20196" windowHeight="7548" tabRatio="882" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -4548,13 +4548,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG40"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="62.44140625" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="10" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="24.33203125" customWidth="1"/>
@@ -23414,7 +23415,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>364</v>
+        <v>394</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>371</v>
@@ -25522,7 +25523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cover line CheckedDiseaseTest
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/CommonCheckerTest.xlsx
+++ b/CloudTest/SampleData/CommonCheckerTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Emr-cloud-api\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" firstSheet="22" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="PT_BYOMEI" sheetId="1" r:id="rId1"/>
@@ -2438,35 +2438,35 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" customWidth="1"/>
-    <col min="9" max="9" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="46.5546875" customWidth="1"/>
-    <col min="28" max="28" width="28.109375" customWidth="1"/>
-    <col min="29" max="29" width="25.33203125" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1"/>
+    <col min="27" max="27" width="46.5703125" customWidth="1"/>
+    <col min="28" max="28" width="28.140625" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" customWidth="1"/>
     <col min="30" max="30" width="21" customWidth="1"/>
-    <col min="31" max="31" width="18.5546875" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
     <col min="32" max="32" width="28" customWidth="1"/>
-    <col min="33" max="33" width="17.5546875" customWidth="1"/>
-    <col min="34" max="34" width="19.6640625" customWidth="1"/>
-    <col min="35" max="35" width="19.109375" customWidth="1"/>
-    <col min="36" max="36" width="16.109375" customWidth="1"/>
-    <col min="37" max="37" width="16.44140625" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" customWidth="1"/>
+    <col min="34" max="34" width="19.7109375" customWidth="1"/>
+    <col min="35" max="35" width="19.140625" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" customWidth="1"/>
+    <col min="37" max="37" width="16.42578125" customWidth="1"/>
     <col min="38" max="38" width="18" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" customWidth="1"/>
-    <col min="40" max="40" width="14.44140625" customWidth="1"/>
-    <col min="41" max="41" width="14.6640625" customWidth="1"/>
-    <col min="42" max="42" width="34.109375" customWidth="1"/>
-    <col min="44" max="44" width="13.6640625" customWidth="1"/>
-    <col min="45" max="45" width="16.44140625" customWidth="1"/>
-    <col min="47" max="47" width="13.6640625" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" customWidth="1"/>
+    <col min="42" max="42" width="34.140625" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" customWidth="1"/>
+    <col min="45" max="45" width="16.42578125" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47">
@@ -4363,12 +4363,12 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="11" max="11" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4514,10 +4514,10 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4553,15 +4553,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4633,17 +4633,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GG41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
+    <sheetView topLeftCell="G27" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="40" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="62.44140625" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="10" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="24.33203125" customWidth="1"/>
+    <col min="154" max="154" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:189">
@@ -24464,15 +24464,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24552,21 +24552,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5546875" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" customWidth="1"/>
-    <col min="16" max="16" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -24698,20 +24698,20 @@
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="40.200000000000003" customHeight="1">
+    <row r="1" spans="1:12" ht="40.15" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -24749,7 +24749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.2" customHeight="1">
+    <row r="2" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A2">
         <v>999</v>
       </c>
@@ -24784,7 +24784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.2" customHeight="1">
+    <row r="3" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A3">
         <v>999</v>
       </c>
@@ -24819,16 +24819,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.2" customHeight="1">
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="16.2" customHeight="1">
+    <row r="5" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="16.2" customHeight="1">
+    <row r="6" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="16.2" customHeight="1">
+    <row r="7" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="F7" s="2"/>
     </row>
   </sheetData>
@@ -24844,19 +24844,19 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -25004,13 +25004,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25074,16 +25074,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -25437,13 +25437,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25579,14 +25579,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -25731,11 +25731,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25784,11 +25784,11 @@
       <selection activeCell="D3" sqref="A3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -25832,10 +25832,10 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25884,9 +25884,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25927,11 +25927,11 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25969,11 +25969,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -26012,18 +26012,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -26253,16 +26253,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -26393,14 +26393,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -26465,16 +26465,16 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -26772,17 +26772,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="33.109375" customWidth="1"/>
-    <col min="9" max="9" width="37.33203125" customWidth="1"/>
-    <col min="10" max="10" width="37.5546875" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="15" max="15" width="25.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -26956,10 +26956,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -26994,10 +26994,10 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -27029,12 +27029,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -27144,19 +27144,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -27296,30 +27296,30 @@
       <selection activeCell="BB18" sqref="BB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
-    <col min="5" max="5" width="39.44140625" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" customWidth="1"/>
-    <col min="32" max="32" width="28.5546875" customWidth="1"/>
-    <col min="33" max="33" width="19.88671875" customWidth="1"/>
-    <col min="35" max="35" width="25.33203125" customWidth="1"/>
-    <col min="36" max="36" width="17.88671875" customWidth="1"/>
-    <col min="40" max="40" width="14.5546875" customWidth="1"/>
-    <col min="42" max="42" width="25.33203125" customWidth="1"/>
-    <col min="43" max="43" width="18.33203125" customWidth="1"/>
-    <col min="44" max="44" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" customWidth="1"/>
+    <col min="32" max="32" width="28.5703125" customWidth="1"/>
+    <col min="33" max="33" width="19.85546875" customWidth="1"/>
+    <col min="35" max="35" width="25.28515625" customWidth="1"/>
+    <col min="36" max="36" width="17.85546875" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" customWidth="1"/>
+    <col min="42" max="42" width="25.28515625" customWidth="1"/>
+    <col min="43" max="43" width="18.28515625" customWidth="1"/>
+    <col min="44" max="44" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -27540,24 +27540,24 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="74.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="34.44140625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -27666,18 +27666,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -27816,17 +27816,17 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.5546875" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>